<commit_message>
Mac: Optimise Area screen for Mac part 1
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/LaSrTiO3.xlsx
+++ b/DATA/UKSAF/LaSrTiO3.xlsx
@@ -405,7 +405,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="4981575" cy="5086350"/>
+    <ext cx="5581650" cy="4076700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -975,13 +975,13 @@
         <v>142.08</v>
       </c>
       <c r="G2" t="n">
-        <v>-2.97859514830634e-11</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
         <v>1321.18</v>
       </c>
       <c r="I2" t="n">
-        <v>1321.18000000003</v>
+        <v>1321.18</v>
       </c>
       <c r="J2" t="n">
         <v>1321.18</v>
@@ -993,7 +993,7 @@
         <v>1321.18</v>
       </c>
       <c r="M2" t="n">
-        <v>1321.18000000003</v>
+        <v>1321.18</v>
       </c>
       <c r="X2" s="16" t="inlineStr">
         <is>
@@ -1007,27 +1007,27 @@
       </c>
       <c r="Z2" s="17" t="inlineStr">
         <is>
-          <t>133.60</t>
+          <t>133.53</t>
         </is>
       </c>
       <c r="AA2" s="17" t="inlineStr">
         <is>
-          <t>3998</t>
+          <t>3892</t>
         </is>
       </c>
       <c r="AB2" s="17" t="inlineStr">
         <is>
-          <t>1.47</t>
+          <t>1.25</t>
         </is>
       </c>
       <c r="AC2" s="17" t="inlineStr">
         <is>
-          <t>22.64</t>
+          <t>20.91</t>
         </is>
       </c>
       <c r="AD2" s="17" t="inlineStr">
         <is>
-          <t>6256</t>
+          <t>5179</t>
         </is>
       </c>
       <c r="AE2" s="17" t="inlineStr"/>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="AH2" s="17" t="inlineStr">
         <is>
-          <t>56.8</t>
+          <t>49.2</t>
         </is>
       </c>
       <c r="AI2" s="17" t="inlineStr">
@@ -1094,13 +1094,13 @@
         <v>141.98</v>
       </c>
       <c r="G3" t="n">
-        <v>-8.594724931754172e-11</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
         <v>1369.78</v>
       </c>
       <c r="I3" t="n">
-        <v>1369.780000000086</v>
+        <v>1369.78</v>
       </c>
       <c r="J3" t="n">
         <v>1369.78</v>
@@ -1112,7 +1112,7 @@
         <v>1369.78</v>
       </c>
       <c r="M3" t="n">
-        <v>1369.780000000086</v>
+        <v>1369.78</v>
       </c>
       <c r="X3" s="19" t="inlineStr"/>
       <c r="Y3" s="20" t="inlineStr"/>
@@ -1153,13 +1153,13 @@
         <v>141.88</v>
       </c>
       <c r="G4" t="n">
-        <v>-2.435172063997015e-10</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>1356.16</v>
       </c>
       <c r="I4" t="n">
-        <v>1356.160000000244</v>
+        <v>1356.16</v>
       </c>
       <c r="J4" t="n">
         <v>1356.16</v>
@@ -1171,7 +1171,7 @@
         <v>1356.16</v>
       </c>
       <c r="M4" t="n">
-        <v>1356.160000000243</v>
+        <v>1356.16</v>
       </c>
       <c r="X4" s="16" t="inlineStr">
         <is>
@@ -1185,27 +1185,27 @@
       </c>
       <c r="Z4" s="17" t="inlineStr">
         <is>
-          <t>135.35</t>
+          <t>135.32</t>
         </is>
       </c>
       <c r="AA4" s="17" t="inlineStr">
         <is>
-          <t>2582</t>
+          <t>2512</t>
         </is>
       </c>
       <c r="AB4" s="17" t="inlineStr">
         <is>
-          <t>1.47</t>
+          <t>1.25</t>
         </is>
       </c>
       <c r="AC4" s="17" t="inlineStr">
         <is>
-          <t>22.64</t>
+          <t>20.91</t>
         </is>
       </c>
       <c r="AD4" s="17" t="inlineStr">
         <is>
-          <t>4040</t>
+          <t>3342</t>
         </is>
       </c>
       <c r="AE4" s="17" t="inlineStr"/>
@@ -1217,17 +1217,17 @@
       </c>
       <c r="AH4" s="17" t="inlineStr">
         <is>
-          <t>36.7</t>
+          <t>31.8</t>
         </is>
       </c>
       <c r="AI4" s="17" t="inlineStr">
         <is>
-          <t>64.6</t>
+          <t>64.5</t>
         </is>
       </c>
       <c r="AJ4" s="17" t="inlineStr">
         <is>
-          <t>1.75</t>
+          <t>1.79</t>
         </is>
       </c>
       <c r="AK4" s="17" t="inlineStr">
@@ -1272,13 +1272,13 @@
         <v>141.78</v>
       </c>
       <c r="G5" t="n">
-        <v>-6.762093107681721e-10</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
         <v>1341.5</v>
       </c>
       <c r="I5" t="n">
-        <v>1341.500000000676</v>
+        <v>1341.5</v>
       </c>
       <c r="J5" t="n">
         <v>1341.5</v>
@@ -1290,7 +1290,7 @@
         <v>1341.5</v>
       </c>
       <c r="M5" t="n">
-        <v>1341.500000000675</v>
+        <v>1341.5</v>
       </c>
       <c r="X5" s="19" t="inlineStr"/>
       <c r="Y5" s="20" t="inlineStr"/>
@@ -1347,13 +1347,13 @@
         <v>141.68</v>
       </c>
       <c r="G6" t="n">
-        <v>-1.842408892116509e-09</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
         <v>1332.29</v>
       </c>
       <c r="I6" t="n">
-        <v>1332.290000001842</v>
+        <v>1332.29</v>
       </c>
       <c r="J6" t="n">
         <v>1332.29</v>
@@ -1365,7 +1365,7 @@
         <v>1332.29</v>
       </c>
       <c r="M6" t="n">
-        <v>1332.290000001839</v>
+        <v>1332.29</v>
       </c>
       <c r="X6" s="16" t="inlineStr">
         <is>
@@ -1379,27 +1379,27 @@
       </c>
       <c r="Z6" s="17" t="inlineStr">
         <is>
-          <t>135.37</t>
+          <t>134.58</t>
         </is>
       </c>
       <c r="AA6" s="17" t="inlineStr">
         <is>
-          <t>270</t>
+          <t>927</t>
         </is>
       </c>
       <c r="AB6" s="17" t="inlineStr">
         <is>
-          <t>1.47</t>
+          <t>1.25</t>
         </is>
       </c>
       <c r="AC6" s="17" t="inlineStr">
         <is>
-          <t>22.64</t>
+          <t>20.91</t>
         </is>
       </c>
       <c r="AD6" s="17" t="inlineStr">
         <is>
-          <t>422</t>
+          <t>1234</t>
         </is>
       </c>
       <c r="AE6" s="17" t="inlineStr"/>
@@ -1411,17 +1411,17 @@
       </c>
       <c r="AH6" s="17" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>11.7</t>
         </is>
       </c>
       <c r="AI6" s="17" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>23.8</t>
         </is>
       </c>
       <c r="AJ6" s="17" t="inlineStr">
         <is>
-          <t>1.77</t>
+          <t>1.05</t>
         </is>
       </c>
       <c r="AK6" s="17" t="inlineStr">
@@ -1446,12 +1446,12 @@
       </c>
       <c r="AO6" s="17" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AP6" s="18" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1466,13 +1466,13 @@
         <v>141.58</v>
       </c>
       <c r="G7" t="n">
-        <v>-4.923322194372304e-09</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
         <v>1338.15</v>
       </c>
       <c r="I7" t="n">
-        <v>1338.150000004923</v>
+        <v>1338.15</v>
       </c>
       <c r="J7" t="n">
         <v>1338.15</v>
@@ -1484,13 +1484,13 @@
         <v>1338.15</v>
       </c>
       <c r="M7" t="n">
-        <v>1338.150000004915</v>
+        <v>1338.15</v>
       </c>
       <c r="X7" s="19" t="inlineStr"/>
       <c r="Y7" s="20" t="inlineStr"/>
       <c r="Z7" s="20" t="inlineStr">
         <is>
-          <t>126.08,142.08</t>
+          <t>A+1.14#0.1</t>
         </is>
       </c>
       <c r="AA7" s="20" t="inlineStr">
@@ -1541,13 +1541,13 @@
         <v>141.48</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.290663931285962e-08</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>1335.29</v>
       </c>
       <c r="I8" t="n">
-        <v>1335.290000012907</v>
+        <v>1335.29</v>
       </c>
       <c r="J8" t="n">
         <v>1335.29</v>
@@ -1559,7 +1559,7 @@
         <v>1335.29</v>
       </c>
       <c r="M8" t="n">
-        <v>1335.290000012883</v>
+        <v>1335.29</v>
       </c>
       <c r="X8" s="16" t="inlineStr">
         <is>
@@ -1573,27 +1573,27 @@
       </c>
       <c r="Z8" s="17" t="inlineStr">
         <is>
-          <t>136.87</t>
+          <t>136.22</t>
         </is>
       </c>
       <c r="AA8" s="17" t="inlineStr">
         <is>
-          <t>185</t>
+          <t>576</t>
         </is>
       </c>
       <c r="AB8" s="17" t="inlineStr">
         <is>
-          <t>1.47</t>
+          <t>1.25</t>
         </is>
       </c>
       <c r="AC8" s="17" t="inlineStr">
         <is>
-          <t>22.64</t>
+          <t>20.91</t>
         </is>
       </c>
       <c r="AD8" s="17" t="inlineStr">
         <is>
-          <t>290</t>
+          <t>767</t>
         </is>
       </c>
       <c r="AE8" s="17" t="inlineStr"/>
@@ -1605,17 +1605,17 @@
       </c>
       <c r="AH8" s="17" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AI8" s="17" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>14.8</t>
         </is>
       </c>
       <c r="AJ8" s="17" t="inlineStr">
         <is>
-          <t>3.27</t>
+          <t>2.69</t>
         </is>
       </c>
       <c r="AK8" s="17" t="inlineStr">
@@ -1640,12 +1640,12 @@
       </c>
       <c r="AO8" s="17" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AP8" s="18" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1660,13 +1660,13 @@
         <v>141.38</v>
       </c>
       <c r="G9" t="n">
-        <v>-3.319223651487846e-08</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
         <v>1341.58</v>
       </c>
       <c r="I9" t="n">
-        <v>1341.580000033192</v>
+        <v>1341.58</v>
       </c>
       <c r="J9" t="n">
         <v>1341.58</v>
@@ -1678,7 +1678,7 @@
         <v>1341.58</v>
       </c>
       <c r="M9" t="n">
-        <v>1341.580000033133</v>
+        <v>1341.58</v>
       </c>
       <c r="X9" s="19" t="inlineStr"/>
       <c r="Y9" s="20" t="inlineStr"/>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="AA9" s="20" t="inlineStr">
         <is>
-          <t>C*0.667#0.05</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AB9" s="20" t="inlineStr">
@@ -1711,7 +1711,7 @@
       <c r="AF9" s="20" t="inlineStr"/>
       <c r="AG9" s="20" t="inlineStr">
         <is>
-          <t>C*1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AH9" s="20" t="inlineStr"/>
@@ -1735,13 +1735,13 @@
         <v>141.28</v>
       </c>
       <c r="G10" t="n">
-        <v>-8.374217941309325e-08</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
         <v>1349.18</v>
       </c>
       <c r="I10" t="n">
-        <v>1349.180000083742</v>
+        <v>1349.18</v>
       </c>
       <c r="J10" t="n">
         <v>1349.18</v>
@@ -1753,7 +1753,7 @@
         <v>1349.18</v>
       </c>
       <c r="M10" t="n">
-        <v>1349.180000083592</v>
+        <v>1349.18</v>
       </c>
     </row>
     <row r="11">
@@ -1767,25 +1767,25 @@
         <v>141.18</v>
       </c>
       <c r="G11" t="n">
-        <v>-2.072722509183222e-07</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>1344.67</v>
       </c>
       <c r="I11" t="n">
-        <v>1344.670000207272</v>
+        <v>1344.67</v>
       </c>
       <c r="J11" t="n">
         <v>1344.67</v>
       </c>
       <c r="K11" t="n">
-        <v>1344.670000000001</v>
+        <v>1344.67</v>
       </c>
       <c r="L11" t="n">
         <v>1344.67</v>
       </c>
       <c r="M11" t="n">
-        <v>1344.670000206901</v>
+        <v>1344.67</v>
       </c>
     </row>
     <row r="12">
@@ -1799,25 +1799,25 @@
         <v>141.08</v>
       </c>
       <c r="G12" t="n">
-        <v>-5.033111847296823e-07</v>
+        <v>-2.273736754432321e-13</v>
       </c>
       <c r="H12" t="n">
         <v>1336.42</v>
       </c>
       <c r="I12" t="n">
-        <v>1336.420000503311</v>
+        <v>1336.42</v>
       </c>
       <c r="J12" t="n">
         <v>1336.42</v>
       </c>
       <c r="K12" t="n">
-        <v>1336.420000000001</v>
+        <v>1336.42</v>
       </c>
       <c r="L12" t="n">
         <v>1336.42</v>
       </c>
       <c r="M12" t="n">
-        <v>1336.42000050241</v>
+        <v>1336.42</v>
       </c>
     </row>
     <row r="13">
@@ -1831,25 +1831,25 @@
         <v>140.98</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.19905780593399e-06</v>
+        <v>-6.821210263296962e-13</v>
       </c>
       <c r="H13" t="n">
         <v>1281.16</v>
       </c>
       <c r="I13" t="n">
-        <v>1281.160001199058</v>
+        <v>1281.160000000001</v>
       </c>
       <c r="J13" t="n">
         <v>1281.16</v>
       </c>
       <c r="K13" t="n">
-        <v>1281.160000000004</v>
+        <v>1281.16</v>
       </c>
       <c r="L13" t="n">
+        <v>1281.16</v>
+      </c>
+      <c r="M13" t="n">
         <v>1281.160000000001</v>
-      </c>
-      <c r="M13" t="n">
-        <v>1281.160001196911</v>
       </c>
     </row>
     <row r="14">
@@ -1863,25 +1863,25 @@
         <v>140.88</v>
       </c>
       <c r="G14" t="n">
-        <v>-2.802602011797717e-06</v>
+        <v>-2.728484105318785e-12</v>
       </c>
       <c r="H14" t="n">
         <v>1323.55</v>
       </c>
       <c r="I14" t="n">
-        <v>1323.550002802602</v>
+        <v>1323.550000000003</v>
       </c>
       <c r="J14" t="n">
         <v>1323.55</v>
       </c>
       <c r="K14" t="n">
-        <v>1323.550000000012</v>
+        <v>1323.55</v>
       </c>
       <c r="L14" t="n">
-        <v>1323.550000000002</v>
+        <v>1323.55</v>
       </c>
       <c r="M14" t="n">
-        <v>1323.55000279758</v>
+        <v>1323.550000000003</v>
       </c>
     </row>
     <row r="15">
@@ -1895,25 +1895,25 @@
         <v>140.78</v>
       </c>
       <c r="G15" t="n">
-        <v>-6.427029120459338e-06</v>
+        <v>-1.000444171950221e-11</v>
       </c>
       <c r="H15" t="n">
         <v>1322.81</v>
       </c>
       <c r="I15" t="n">
-        <v>1322.810006427029</v>
+        <v>1322.81000000001</v>
       </c>
       <c r="J15" t="n">
         <v>1322.81</v>
       </c>
       <c r="K15" t="n">
-        <v>1322.810000000038</v>
+        <v>1322.81</v>
       </c>
       <c r="L15" t="n">
-        <v>1322.810000000005</v>
+        <v>1322.81</v>
       </c>
       <c r="M15" t="n">
-        <v>1322.810006415502</v>
+        <v>1322.81000000001</v>
       </c>
     </row>
     <row r="16">
@@ -1927,25 +1927,25 @@
         <v>140.68</v>
       </c>
       <c r="G16" t="n">
-        <v>-1.446094324819569e-05</v>
+        <v>-3.728928277269006e-11</v>
       </c>
       <c r="H16" t="n">
         <v>1352.14</v>
       </c>
       <c r="I16" t="n">
-        <v>1352.140014460943</v>
+        <v>1352.140000000037</v>
       </c>
       <c r="J16" t="n">
         <v>1352.14</v>
       </c>
       <c r="K16" t="n">
-        <v>1352.140000000114</v>
+        <v>1352.14</v>
       </c>
       <c r="L16" t="n">
-        <v>1352.140000000015</v>
+        <v>1352.14</v>
       </c>
       <c r="M16" t="n">
-        <v>1352.140014434975</v>
+        <v>1352.140000000037</v>
       </c>
     </row>
     <row r="17">
@@ -1959,25 +1959,25 @@
         <v>140.58</v>
       </c>
       <c r="G17" t="n">
-        <v>-3.192498002135835e-05</v>
+        <v>-1.336957211606205e-10</v>
       </c>
       <c r="H17" t="n">
         <v>1304.84</v>
       </c>
       <c r="I17" t="n">
-        <v>1304.84003192498</v>
+        <v>1304.840000000134</v>
       </c>
       <c r="J17" t="n">
         <v>1304.84</v>
       </c>
       <c r="K17" t="n">
-        <v>1304.840000000335</v>
+        <v>1304.84</v>
       </c>
       <c r="L17" t="n">
-        <v>1304.840000000043</v>
+        <v>1304.84</v>
       </c>
       <c r="M17" t="n">
-        <v>1304.840031867556</v>
+        <v>1304.840000000134</v>
       </c>
     </row>
     <row r="18">
@@ -1991,25 +1991,25 @@
         <v>140.48</v>
       </c>
       <c r="G18" t="n">
-        <v>-6.915482731528755e-05</v>
+        <v>-4.677076503867283e-10</v>
       </c>
       <c r="H18" t="n">
         <v>1296.85</v>
       </c>
       <c r="I18" t="n">
-        <v>1296.850069154827</v>
+        <v>1296.850000000468</v>
       </c>
       <c r="J18" t="n">
         <v>1296.85</v>
       </c>
       <c r="K18" t="n">
-        <v>1296.850000000971</v>
+        <v>1296.85</v>
       </c>
       <c r="L18" t="n">
-        <v>1296.850000000125</v>
+        <v>1296.85</v>
       </c>
       <c r="M18" t="n">
-        <v>1296.850069030162</v>
+        <v>1296.850000000467</v>
       </c>
     </row>
     <row r="19">
@@ -2023,25 +2023,25 @@
         <v>140.38</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.000146988191318087</v>
+        <v>-1.591388354427181e-09</v>
       </c>
       <c r="H19" t="n">
         <v>1297.71</v>
       </c>
       <c r="I19" t="n">
-        <v>1297.710146988191</v>
+        <v>1297.710000001591</v>
       </c>
       <c r="J19" t="n">
         <v>1297.71</v>
       </c>
       <c r="K19" t="n">
-        <v>1297.710000002759</v>
+        <v>1297.71</v>
       </c>
       <c r="L19" t="n">
-        <v>1297.710000000355</v>
+        <v>1297.71</v>
       </c>
       <c r="M19" t="n">
-        <v>1297.710146722433</v>
+        <v>1297.71000000159</v>
       </c>
     </row>
     <row r="20">
@@ -2055,25 +2055,25 @@
         <v>140.28</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.0003065636349219858</v>
+        <v>-5.269839675747789e-09</v>
       </c>
       <c r="H20" t="n">
         <v>1346.66</v>
       </c>
       <c r="I20" t="n">
-        <v>1346.660306563635</v>
+        <v>1346.66000000527</v>
       </c>
       <c r="J20" t="n">
         <v>1346.66</v>
       </c>
       <c r="K20" t="n">
-        <v>1346.660000007693</v>
+        <v>1346.66</v>
       </c>
       <c r="L20" t="n">
-        <v>1346.660000000985</v>
+        <v>1346.66</v>
       </c>
       <c r="M20" t="n">
-        <v>1346.660306007183</v>
+        <v>1346.660000005266</v>
       </c>
     </row>
     <row r="21">
@@ -2087,25 +2087,25 @@
         <v>140.18</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.0006274037209550443</v>
+        <v>-1.698344931355678e-08</v>
       </c>
       <c r="H21" t="n">
         <v>1293.78</v>
       </c>
       <c r="I21" t="n">
-        <v>1293.780627403721</v>
+        <v>1293.780000016983</v>
       </c>
       <c r="J21" t="n">
         <v>1293.78</v>
       </c>
       <c r="K21" t="n">
-        <v>1293.780000021037</v>
+        <v>1293.780000000001</v>
       </c>
       <c r="L21" t="n">
-        <v>1293.780000002684</v>
+        <v>1293.78</v>
       </c>
       <c r="M21" t="n">
-        <v>1293.780626258954</v>
+        <v>1293.78000001697</v>
       </c>
     </row>
     <row r="22">
@@ -2119,25 +2119,25 @@
         <v>140.08</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.001260002931076087</v>
+        <v>-5.326637619873509e-08</v>
       </c>
       <c r="H22" t="n">
         <v>1294.58</v>
       </c>
       <c r="I22" t="n">
-        <v>1294.581260002931</v>
+        <v>1294.580000053266</v>
       </c>
       <c r="J22" t="n">
         <v>1294.58</v>
       </c>
       <c r="K22" t="n">
-        <v>1294.580000056435</v>
+        <v>1294.580000000003</v>
       </c>
       <c r="L22" t="n">
-        <v>1294.580000007172</v>
+        <v>1294.58</v>
       </c>
       <c r="M22" t="n">
-        <v>1294.581257687979</v>
+        <v>1294.580000053223</v>
       </c>
     </row>
     <row r="23">
@@ -2151,25 +2151,25 @@
         <v>139.98</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.002483152424474611</v>
+        <v>-1.625903678359464e-07</v>
       </c>
       <c r="H23" t="n">
         <v>1282.76</v>
       </c>
       <c r="I23" t="n">
-        <v>1282.762483152424</v>
+        <v>1282.76000016259</v>
       </c>
       <c r="J23" t="n">
         <v>1282.76</v>
       </c>
       <c r="K23" t="n">
-        <v>1282.760000148516</v>
+        <v>1282.760000000012</v>
       </c>
       <c r="L23" t="n">
-        <v>1282.760000018803</v>
+        <v>1282.76</v>
       </c>
       <c r="M23" t="n">
-        <v>1282.762478548349</v>
+        <v>1282.760000162455</v>
       </c>
     </row>
     <row r="24">
@@ -2183,25 +2183,25 @@
         <v>139.88</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.004802322629757327</v>
+        <v>-4.830196758121019e-07</v>
       </c>
       <c r="H24" t="n">
         <v>1291.45</v>
       </c>
       <c r="I24" t="n">
-        <v>1291.45480232263</v>
+        <v>1291.45000048302</v>
       </c>
       <c r="J24" t="n">
         <v>1291.45</v>
       </c>
       <c r="K24" t="n">
-        <v>1291.450000383411</v>
+        <v>1291.450000000044</v>
       </c>
       <c r="L24" t="n">
-        <v>1291.450000048356</v>
+        <v>1291.45</v>
       </c>
       <c r="M24" t="n">
-        <v>1291.454793310556</v>
+        <v>1291.450000482608</v>
       </c>
     </row>
     <row r="25">
@@ -2215,25 +2215,25 @@
         <v>139.78</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.009114302045873046</v>
+        <v>-1.396616198690026e-06</v>
       </c>
       <c r="H25" t="n">
         <v>1275.21</v>
       </c>
       <c r="I25" t="n">
-        <v>1275.219114302046</v>
+        <v>1275.210001396616</v>
       </c>
       <c r="J25" t="n">
         <v>1275.21</v>
       </c>
       <c r="K25" t="n">
-        <v>1275.210000971035</v>
+        <v>1275.210000000162</v>
       </c>
       <c r="L25" t="n">
-        <v>1275.210000122</v>
+        <v>1275.21</v>
       </c>
       <c r="M25" t="n">
-        <v>1275.219096925031</v>
+        <v>1275.210001395391</v>
       </c>
     </row>
     <row r="26">
@@ -2247,25 +2247,25 @@
         <v>139.68</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.01697565770064102</v>
+        <v>-3.930484808734036e-06</v>
       </c>
       <c r="H26" t="n">
         <v>1311.33</v>
       </c>
       <c r="I26" t="n">
-        <v>1311.346975657701</v>
+        <v>1311.330003930485</v>
       </c>
       <c r="J26" t="n">
         <v>1311.33</v>
       </c>
       <c r="K26" t="n">
-        <v>1311.330002412642</v>
+        <v>1311.330000000583</v>
       </c>
       <c r="L26" t="n">
-        <v>1311.330000301964</v>
+        <v>1311.33</v>
       </c>
       <c r="M26" t="n">
-        <v>1311.346942615031</v>
+        <v>1311.330003926911</v>
       </c>
     </row>
     <row r="27">
@@ -2279,25 +2279,25 @@
         <v>139.58</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.03102891483899839</v>
+        <v>-1.0766816103569e-05</v>
       </c>
       <c r="H27" t="n">
         <v>1287.86</v>
       </c>
       <c r="I27" t="n">
-        <v>1287.891028914839</v>
+        <v>1287.860010766816</v>
       </c>
       <c r="J27" t="n">
         <v>1287.86</v>
       </c>
       <c r="K27" t="n">
-        <v>1287.860005880953</v>
+        <v>1287.860000002038</v>
       </c>
       <c r="L27" t="n">
-        <v>1287.860000733247</v>
+        <v>1287.86</v>
       </c>
       <c r="M27" t="n">
-        <v>1287.890966868805</v>
+        <v>1287.860010756586</v>
       </c>
     </row>
     <row r="28">
@@ -2311,25 +2311,25 @@
         <v>139.48</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.05566053609118171</v>
+        <v>-2.870887169592606e-05</v>
       </c>
       <c r="H28" t="n">
         <v>1305.54</v>
       </c>
       <c r="I28" t="n">
-        <v>1305.595660536091</v>
+        <v>1305.540028708872</v>
       </c>
       <c r="J28" t="n">
         <v>1305.54</v>
       </c>
       <c r="K28" t="n">
-        <v>1305.540014063991</v>
+        <v>1305.540000006934</v>
       </c>
       <c r="L28" t="n">
-        <v>1305.540001746843</v>
+        <v>1305.54</v>
       </c>
       <c r="M28" t="n">
-        <v>1305.595545297828</v>
+        <v>1305.540028680093</v>
       </c>
     </row>
     <row r="29">
@@ -2343,25 +2343,25 @@
         <v>139.38</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.09798757247085632</v>
+        <v>-7.451582587236771e-05</v>
       </c>
       <c r="H29" t="n">
         <v>1286.85</v>
       </c>
       <c r="I29" t="n">
-        <v>1286.947987572471</v>
+        <v>1286.850074515826</v>
       </c>
       <c r="J29" t="n">
+        <v>1286.85</v>
+      </c>
+      <c r="K29" t="n">
+        <v>1286.850000022964</v>
+      </c>
+      <c r="L29" t="n">
         <v>1286.850000000001</v>
       </c>
-      <c r="K29" t="n">
-        <v>1286.850032997804</v>
-      </c>
-      <c r="L29" t="n">
-        <v>1286.850004082955</v>
-      </c>
       <c r="M29" t="n">
-        <v>1286.947775472868</v>
+        <v>1286.850074436169</v>
       </c>
     </row>
     <row r="30">
@@ -2375,25 +2375,25 @@
         <v>139.28</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.1692921933165508</v>
+        <v>-0.0001882784838471707</v>
       </c>
       <c r="H30" t="n">
         <v>1284.54</v>
       </c>
       <c r="I30" t="n">
-        <v>1284.709292193317</v>
+        <v>1284.540188278484</v>
       </c>
       <c r="J30" t="n">
-        <v>1284.540000000003</v>
+        <v>1284.54</v>
       </c>
       <c r="K30" t="n">
-        <v>1284.540075960338</v>
+        <v>1284.540000074007</v>
       </c>
       <c r="L30" t="n">
-        <v>1284.540009363165</v>
+        <v>1284.540000000002</v>
       </c>
       <c r="M30" t="n">
-        <v>1284.708904533136</v>
+        <v>1284.540188061246</v>
       </c>
     </row>
     <row r="31">
@@ -2407,25 +2407,25 @@
         <v>139.18</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.2870395045492842</v>
+        <v>-0.0004631152414731332</v>
       </c>
       <c r="H31" t="n">
         <v>1296.58</v>
       </c>
       <c r="I31" t="n">
-        <v>1296.867039504549</v>
+        <v>1296.580463115241</v>
       </c>
       <c r="J31" t="n">
-        <v>1296.580000000011</v>
+        <v>1296.58</v>
       </c>
       <c r="K31" t="n">
-        <v>1296.580171563152</v>
+        <v>1296.580000232111</v>
       </c>
       <c r="L31" t="n">
-        <v>1296.580021067261</v>
+        <v>1296.580000000009</v>
       </c>
       <c r="M31" t="n">
-        <v>1296.866334348172</v>
+        <v>1296.580462530861</v>
       </c>
     </row>
     <row r="32">
@@ -2439,25 +2439,25 @@
         <v>139.08</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.4776151641183333</v>
+        <v>-0.00110899661399344</v>
       </c>
       <c r="H32" t="n">
         <v>1288.78</v>
       </c>
       <c r="I32" t="n">
-        <v>1289.257615164118</v>
+        <v>1288.781108996614</v>
       </c>
       <c r="J32" t="n">
-        <v>1288.780000000033</v>
+        <v>1288.78</v>
       </c>
       <c r="K32" t="n">
-        <v>1288.780380195049</v>
+        <v>1288.780000708485</v>
       </c>
       <c r="L32" t="n">
-        <v>1288.780046509406</v>
+        <v>1288.780000000036</v>
       </c>
       <c r="M32" t="n">
-        <v>1289.256335857829</v>
+        <v>1288.781107444691</v>
       </c>
     </row>
     <row r="33">
@@ -2471,25 +2471,25 @@
         <v>138.98</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.7798927551314137</v>
+        <v>-0.002585477009233728</v>
       </c>
       <c r="H33" t="n">
         <v>1262.37</v>
       </c>
       <c r="I33" t="n">
-        <v>1263.149892755131</v>
+        <v>1262.372585477009</v>
       </c>
       <c r="J33" t="n">
-        <v>1262.370000000101</v>
+        <v>1262.37</v>
       </c>
       <c r="K33" t="n">
-        <v>1262.37082669307</v>
+        <v>1262.370002104708</v>
       </c>
       <c r="L33" t="n">
-        <v>1262.370100746723</v>
+        <v>1262.370000000129</v>
       </c>
       <c r="M33" t="n">
-        <v>1263.147573563051</v>
+        <v>1262.372581406295</v>
       </c>
     </row>
     <row r="34">
@@ -2503,25 +2503,25 @@
         <v>138.88</v>
       </c>
       <c r="G34" t="n">
-        <v>-1.249671140608825</v>
+        <v>-0.005868631508519684</v>
       </c>
       <c r="H34" t="n">
         <v>1298.36</v>
       </c>
       <c r="I34" t="n">
-        <v>1299.609671140609</v>
+        <v>1298.365868631508</v>
       </c>
       <c r="J34" t="n">
-        <v>1298.360000000303</v>
+        <v>1298.36</v>
       </c>
       <c r="K34" t="n">
-        <v>1298.361763793038</v>
+        <v>1298.360006085456</v>
       </c>
       <c r="L34" t="n">
-        <v>1298.360214135443</v>
+        <v>1298.360000000457</v>
       </c>
       <c r="M34" t="n">
-        <v>1299.605464084018</v>
+        <v>1298.365858084522</v>
       </c>
     </row>
     <row r="35">
@@ -2535,25 +2535,25 @@
         <v>138.78</v>
       </c>
       <c r="G35" t="n">
-        <v>-1.964892568323194</v>
+        <v>-0.01296984323153083</v>
       </c>
       <c r="H35" t="n">
         <v>1231.15</v>
       </c>
       <c r="I35" t="n">
-        <v>1233.114892568323</v>
+        <v>1231.162969843232</v>
       </c>
       <c r="J35" t="n">
-        <v>1231.150000000885</v>
+        <v>1231.15</v>
       </c>
       <c r="K35" t="n">
-        <v>1231.153692550472</v>
+        <v>1231.150017125696</v>
       </c>
       <c r="L35" t="n">
-        <v>1231.150446605078</v>
+        <v>1231.150000001573</v>
       </c>
       <c r="M35" t="n">
-        <v>1233.107250509573</v>
+        <v>1231.162942860131</v>
       </c>
     </row>
     <row r="36">
@@ -2567,25 +2567,25 @@
         <v>138.68</v>
       </c>
       <c r="G36" t="n">
-        <v>-3.031349624708355</v>
+        <v>-0.02790935212146906</v>
       </c>
       <c r="H36" t="n">
         <v>1288.75</v>
       </c>
       <c r="I36" t="n">
-        <v>1291.781349624708</v>
+        <v>1288.777909352121</v>
       </c>
       <c r="J36" t="n">
-        <v>1288.750000002541</v>
+        <v>1288.75</v>
       </c>
       <c r="K36" t="n">
-        <v>1288.757585610795</v>
+        <v>1288.750046910666</v>
       </c>
       <c r="L36" t="n">
-        <v>1288.750913999554</v>
+        <v>1288.750000005266</v>
       </c>
       <c r="M36" t="n">
-        <v>1291.767450030729</v>
+        <v>1288.77784123671</v>
       </c>
     </row>
     <row r="37">
@@ -2599,25 +2599,25 @@
         <v>138.58</v>
       </c>
       <c r="G37" t="n">
-        <v>-4.588309309000579</v>
+        <v>-0.05847852893680283</v>
       </c>
       <c r="H37" t="n">
         <v>1264.45</v>
       </c>
       <c r="I37" t="n">
-        <v>1269.038309309001</v>
+        <v>1264.508478528937</v>
       </c>
       <c r="J37" t="n">
-        <v>1264.450000007151</v>
+        <v>1264.45</v>
       </c>
       <c r="K37" t="n">
-        <v>1264.465291477876</v>
+        <v>1264.450125077075</v>
       </c>
       <c r="L37" t="n">
-        <v>1264.451835544618</v>
+        <v>1264.450000017158</v>
       </c>
       <c r="M37" t="n">
-        <v>1269.013017113105</v>
+        <v>1264.508309039189</v>
       </c>
     </row>
     <row r="38">
@@ -2631,25 +2631,25 @@
         <v>138.48</v>
       </c>
       <c r="G38" t="n">
-        <v>-6.813140225260213</v>
+        <v>-0.1193130725389437</v>
       </c>
       <c r="H38" t="n">
         <v>1303.52</v>
       </c>
       <c r="I38" t="n">
-        <v>1310.33314022526</v>
+        <v>1303.639313072539</v>
       </c>
       <c r="J38" t="n">
-        <v>1303.520000019746</v>
+        <v>1303.52</v>
       </c>
       <c r="K38" t="n">
-        <v>1303.550249079376</v>
+        <v>1303.520324624405</v>
       </c>
       <c r="L38" t="n">
-        <v>1303.523617340833</v>
+        <v>1303.5200000544</v>
       </c>
       <c r="M38" t="n">
-        <v>1310.287165922625</v>
+        <v>1303.638897875772</v>
       </c>
     </row>
     <row r="39">
@@ -2663,25 +2663,25 @@
         <v>138.38</v>
       </c>
       <c r="G39" t="n">
-        <v>-9.923668636016146</v>
+        <v>-0.2370478884881777</v>
       </c>
       <c r="H39" t="n">
         <v>1312.96</v>
       </c>
       <c r="I39" t="n">
-        <v>1322.883668636016</v>
+        <v>1313.197047888488</v>
       </c>
       <c r="J39" t="n">
-        <v>1312.960000053481</v>
+        <v>1312.960000000001</v>
       </c>
       <c r="K39" t="n">
-        <v>1313.018720127006</v>
+        <v>1312.960820155987</v>
       </c>
       <c r="L39" t="n">
-        <v>1312.966995642433</v>
+        <v>1312.960000167861</v>
       </c>
       <c r="M39" t="n">
-        <v>1322.800349217209</v>
+        <v>1313.196047881772</v>
       </c>
     </row>
     <row r="40">
@@ -2695,25 +2695,25 @@
         <v>138.28</v>
       </c>
       <c r="G40" t="n">
-        <v>-14.17669646134868</v>
+        <v>-0.4586168524917866</v>
       </c>
       <c r="H40" t="n">
         <v>1276.13</v>
       </c>
       <c r="I40" t="n">
-        <v>1290.306696461349</v>
+        <v>1276.588616852492</v>
       </c>
       <c r="J40" t="n">
-        <v>1276.130000142099</v>
+        <v>1276.130000000005</v>
       </c>
       <c r="K40" t="n">
-        <v>1276.241861680857</v>
+        <v>1276.132017148477</v>
       </c>
       <c r="L40" t="n">
-        <v>1276.143276593288</v>
+        <v>1276.130000504103</v>
       </c>
       <c r="M40" t="n">
-        <v>1290.156471205217</v>
+        <v>1276.586251949723</v>
       </c>
     </row>
     <row r="41">
@@ -2727,25 +2727,25 @@
         <v>138.18</v>
       </c>
       <c r="G41" t="n">
-        <v>-19.8610241466572</v>
+        <v>-0.8640451512985692</v>
       </c>
       <c r="H41" t="n">
         <v>1283.01</v>
       </c>
       <c r="I41" t="n">
-        <v>1302.871024146657</v>
+        <v>1283.874045151299</v>
       </c>
       <c r="J41" t="n">
-        <v>1283.010000370379</v>
+        <v>1283.01000000002</v>
       </c>
       <c r="K41" t="n">
-        <v>1283.219122813703</v>
+        <v>1283.014829689348</v>
       </c>
       <c r="L41" t="n">
-        <v>1283.034727059774</v>
+        <v>1283.010001473408</v>
       </c>
       <c r="M41" t="n">
-        <v>1302.602142760997</v>
+        <v>1283.868560675641</v>
       </c>
     </row>
     <row r="42">
@@ -2759,25 +2759,25 @@
         <v>138.08</v>
       </c>
       <c r="G42" t="n">
-        <v>-53.89361732972884</v>
+        <v>-28.19525340734094</v>
       </c>
       <c r="H42" t="n">
         <v>1278.08</v>
       </c>
       <c r="I42" t="n">
-        <v>1305.363617329729</v>
+        <v>1279.665253407341</v>
       </c>
       <c r="J42" t="n">
-        <v>1278.080000947056</v>
+        <v>1278.080000000077</v>
       </c>
       <c r="K42" t="n">
-        <v>1278.463664675242</v>
+        <v>1278.091257799674</v>
       </c>
       <c r="L42" t="n">
-        <v>1278.125194889607</v>
+        <v>1278.080004191552</v>
       </c>
       <c r="M42" t="n">
-        <v>1304.886844225679</v>
+        <v>1279.652794920835</v>
       </c>
     </row>
     <row r="43">
@@ -2791,25 +2791,25 @@
         <v>137.98</v>
       </c>
       <c r="G43" t="n">
-        <v>-46.21845308062075</v>
+        <v>-12.30227986857267</v>
       </c>
       <c r="H43" t="n">
         <v>1277.73</v>
       </c>
       <c r="I43" t="n">
-        <v>1314.478453080621</v>
+        <v>1280.562279868573</v>
       </c>
       <c r="J43" t="n">
-        <v>1277.730002375685</v>
+        <v>1277.730000000286</v>
       </c>
       <c r="K43" t="n">
-        <v>1278.42077265643</v>
+        <v>1277.755547757501</v>
       </c>
       <c r="L43" t="n">
-        <v>1277.811066110343</v>
+        <v>1277.730011606178</v>
       </c>
       <c r="M43" t="n">
-        <v>1313.642458228095</v>
+        <v>1280.534587626218</v>
       </c>
     </row>
     <row r="44">
@@ -2823,25 +2823,25 @@
         <v>137.88</v>
       </c>
       <c r="G44" t="n">
-        <v>-11.74927892575238</v>
+        <v>31.85230568361339</v>
       </c>
       <c r="H44" t="n">
         <v>1277.74</v>
       </c>
       <c r="I44" t="n">
-        <v>1326.269278925752</v>
+        <v>1282.667694316387</v>
       </c>
       <c r="J44" t="n">
-        <v>1277.740005846477</v>
+        <v>1277.740000001025</v>
       </c>
       <c r="K44" t="n">
-        <v>1278.960538354746</v>
+        <v>1277.796445251128</v>
       </c>
       <c r="L44" t="n">
-        <v>1277.882699338781</v>
+        <v>1277.740031280991</v>
       </c>
       <c r="M44" t="n">
-        <v>1324.821988205624</v>
+        <v>1282.607517593877</v>
       </c>
     </row>
     <row r="45">
@@ -2855,25 +2855,25 @@
         <v>137.78</v>
       </c>
       <c r="G45" t="n">
-        <v>-26.22011543102803</v>
+        <v>28.27143968879227</v>
       </c>
       <c r="H45" t="n">
         <v>1277.73</v>
       </c>
       <c r="I45" t="n">
-        <v>1340.570115431028</v>
+        <v>1286.078560311208</v>
       </c>
       <c r="J45" t="n">
-        <v>1277.730014115649</v>
+        <v>1277.730000003573</v>
       </c>
       <c r="K45" t="n">
-        <v>1279.846399038339</v>
+        <v>1277.851418726763</v>
       </c>
       <c r="L45" t="n">
-        <v>1277.976509318631</v>
+        <v>1277.730082066001</v>
       </c>
       <c r="M45" t="n">
-        <v>1338.099530104346</v>
+        <v>1285.950813532466</v>
       </c>
     </row>
     <row r="46">
@@ -2887,25 +2887,25 @@
         <v>137.68</v>
       </c>
       <c r="G46" t="n">
-        <v>4.079299731895617</v>
+        <v>70.1171101748655</v>
       </c>
       <c r="H46" t="n">
         <v>1277.7</v>
       </c>
       <c r="I46" t="n">
-        <v>1357.510700268104</v>
+        <v>1291.472889825134</v>
       </c>
       <c r="J46" t="n">
-        <v>1277.700033436307</v>
+        <v>1277.700000012126</v>
       </c>
       <c r="K46" t="n">
-        <v>1281.301358985457</v>
+        <v>1277.954292198687</v>
       </c>
       <c r="L46" t="n">
-        <v>1278.117893373007</v>
+        <v>1277.700209581092</v>
       </c>
       <c r="M46" t="n">
-        <v>1353.356667526453</v>
+        <v>1291.208131825697</v>
       </c>
     </row>
     <row r="47">
@@ -2919,25 +2919,25 @@
         <v>137.58</v>
       </c>
       <c r="G47" t="n">
-        <v>-57.70768767957202</v>
+        <v>19.6458888323416</v>
       </c>
       <c r="H47" t="n">
         <v>1277.65</v>
       </c>
       <c r="I47" t="n">
-        <v>1377.127687679572</v>
+        <v>1299.774111167658</v>
       </c>
       <c r="J47" t="n">
-        <v>1277.650077706299</v>
+        <v>1277.650000040046</v>
       </c>
       <c r="K47" t="n">
-        <v>1283.663759163622</v>
+        <v>1278.168526847119</v>
       </c>
       <c r="L47" t="n">
-        <v>1278.345192873588</v>
+        <v>1277.650521028371</v>
       </c>
       <c r="M47" t="n">
-        <v>1370.254029192014</v>
+        <v>1299.238686010642</v>
       </c>
     </row>
     <row r="48">
@@ -2951,25 +2951,25 @@
         <v>137.48</v>
       </c>
       <c r="G48" t="n">
-        <v>-94.34523357054741</v>
+        <v>-7.143014042426103</v>
       </c>
       <c r="H48" t="n">
         <v>1277.6</v>
       </c>
       <c r="I48" t="n">
-        <v>1399.405233570547</v>
+        <v>1312.203014042426</v>
       </c>
       <c r="J48" t="n">
-        <v>1277.600177183987</v>
+        <v>1277.600000128706</v>
       </c>
       <c r="K48" t="n">
-        <v>1287.45413373546</v>
+        <v>1278.629431039949</v>
       </c>
       <c r="L48" t="n">
-        <v>1278.73483709202</v>
+        <v>1277.601260971052</v>
       </c>
       <c r="M48" t="n">
-        <v>1388.219929656147</v>
+        <v>1311.146901461421</v>
       </c>
     </row>
     <row r="49">
@@ -2983,25 +2983,25 @@
         <v>137.38</v>
       </c>
       <c r="G49" t="n">
-        <v>-29.16902897607793</v>
+        <v>64.88707703559726</v>
       </c>
       <c r="H49" t="n">
         <v>1277.57</v>
       </c>
       <c r="I49" t="n">
-        <v>1424.319028976078</v>
+        <v>1330.262922964403</v>
       </c>
       <c r="J49" t="n">
-        <v>1277.570396399407</v>
+        <v>1277.570000402571</v>
       </c>
       <c r="K49" t="n">
-        <v>1293.413766592244</v>
+        <v>1279.559765447402</v>
       </c>
       <c r="L49" t="n">
-        <v>1279.387704338837</v>
+        <v>1277.572970959518</v>
       </c>
       <c r="M49" t="n">
-        <v>1406.429479409646</v>
+        <v>1328.231851761161</v>
       </c>
     </row>
     <row r="50">
@@ -3015,25 +3015,25 @@
         <v>137.28</v>
       </c>
       <c r="G50" t="n">
-        <v>-69.74404425464763</v>
+        <v>26.50780021173068</v>
       </c>
       <c r="H50" t="n">
         <v>1277.52</v>
       </c>
       <c r="I50" t="n">
-        <v>1451.894044254648</v>
+        <v>1355.642199788269</v>
       </c>
       <c r="J50" t="n">
-        <v>1277.520870145488</v>
+        <v>1277.520001225461</v>
       </c>
       <c r="K50" t="n">
-        <v>1302.513779070279</v>
+        <v>1281.264278502103</v>
       </c>
       <c r="L50" t="n">
-        <v>1280.376527770728</v>
+        <v>1277.526814730349</v>
       </c>
       <c r="M50" t="n">
-        <v>1423.78573830978</v>
+        <v>1351.834977514774</v>
       </c>
     </row>
     <row r="51">
@@ -3047,25 +3047,25 @@
         <v>137.18</v>
       </c>
       <c r="G51" t="n">
-        <v>-59.97676156347165</v>
+        <v>32.27903860485549</v>
       </c>
       <c r="H51" t="n">
         <v>1277.43</v>
       </c>
       <c r="I51" t="n">
-        <v>1482.456761563472</v>
+        <v>1390.200961395145</v>
       </c>
       <c r="J51" t="n">
-        <v>1277.431874179565</v>
+        <v>1277.430003630649</v>
       </c>
       <c r="K51" t="n">
-        <v>1316.110694547229</v>
+        <v>1284.289133404753</v>
       </c>
       <c r="L51" t="n">
-        <v>1281.833845990793</v>
+        <v>1277.44521850639</v>
       </c>
       <c r="M51" t="n">
-        <v>1439.088217144659</v>
+        <v>1383.24687807375</v>
       </c>
     </row>
     <row r="52">
@@ -3079,25 +3079,25 @@
         <v>137.08</v>
       </c>
       <c r="G52" t="n">
-        <v>-54.24743458920648</v>
+        <v>26.78136281701677</v>
       </c>
       <c r="H52" t="n">
         <v>1277.33</v>
       </c>
       <c r="I52" t="n">
-        <v>1516.877434589207</v>
+        <v>1435.848637182983</v>
       </c>
       <c r="J52" t="n">
-        <v>1277.333960965218</v>
+        <v>1277.33001046912</v>
       </c>
       <c r="K52" t="n">
-        <v>1336.050280834115</v>
+        <v>1289.561118258781</v>
       </c>
       <c r="L52" t="n">
-        <v>1283.989538489397</v>
+        <v>1277.363088418402</v>
       </c>
       <c r="M52" t="n">
-        <v>1451.193402974732</v>
+        <v>1423.474653768738</v>
       </c>
     </row>
     <row r="53">
@@ -3111,25 +3111,25 @@
         <v>136.98</v>
       </c>
       <c r="G53" t="n">
-        <v>-30.12914168719453</v>
+        <v>32.31281859236947</v>
       </c>
       <c r="H53" t="n">
         <v>1277.2</v>
       </c>
       <c r="I53" t="n">
-        <v>1556.689141687194</v>
+        <v>1494.24718140763</v>
       </c>
       <c r="J53" t="n">
-        <v>1277.208214313717</v>
+        <v>1277.200029382684</v>
       </c>
       <c r="K53" t="n">
-        <v>1364.626116737397</v>
+        <v>1298.427785062185</v>
       </c>
       <c r="L53" t="n">
-        <v>1287.076404319507</v>
+        <v>1277.270043411841</v>
       </c>
       <c r="M53" t="n">
-        <v>1459.069145749753</v>
+        <v>1472.803018380537</v>
       </c>
     </row>
     <row r="54">
@@ -3143,25 +3143,25 @@
         <v>136.88</v>
       </c>
       <c r="G54" t="n">
-        <v>-2.632748809111263</v>
+        <v>35.0200276101184</v>
       </c>
       <c r="H54" t="n">
         <v>1277.02</v>
       </c>
       <c r="I54" t="n">
-        <v>1604.312748809111</v>
+        <v>1566.659972389882</v>
       </c>
       <c r="J54" t="n">
-        <v>1277.036715972009</v>
+        <v>1277.020080268</v>
       </c>
       <c r="K54" t="n">
-        <v>1404.653167756159</v>
+        <v>1312.871881238811</v>
       </c>
       <c r="L54" t="n">
-        <v>1291.38159074944</v>
+        <v>1277.164360784531</v>
       </c>
       <c r="M54" t="n">
-        <v>1461.993886136954</v>
+        <v>1530.475114229045</v>
       </c>
     </row>
     <row r="55">
@@ -3175,25 +3175,25 @@
         <v>136.78</v>
       </c>
       <c r="G55" t="n">
-        <v>-12.83630537823296</v>
+        <v>-3.522030516444602</v>
       </c>
       <c r="H55" t="n">
         <v>1276.79</v>
       </c>
       <c r="I55" t="n">
-        <v>1663.146305378233</v>
+        <v>1653.832030516445</v>
       </c>
       <c r="J55" t="n">
-        <v>1276.823380385617</v>
+        <v>1276.790213440897</v>
       </c>
       <c r="K55" t="n">
-        <v>1459.450608349626</v>
+        <v>1335.700463795401</v>
       </c>
       <c r="L55" t="n">
-        <v>1297.26106608329</v>
+        <v>1277.079681559654</v>
       </c>
       <c r="M55" t="n">
-        <v>1459.687714272684</v>
+        <v>1594.397151267937</v>
       </c>
     </row>
     <row r="56">
@@ -3207,25 +3207,25 @@
         <v>136.68</v>
       </c>
       <c r="G56" t="n">
-        <v>-2.968803858029105</v>
+        <v>-21.48987226331519</v>
       </c>
       <c r="H56" t="n">
         <v>1276.52</v>
       </c>
       <c r="I56" t="n">
-        <v>1737.458803858029</v>
+        <v>1755.979872263315</v>
       </c>
       <c r="J56" t="n">
-        <v>1276.585412255223</v>
+        <v>1276.520552473716</v>
       </c>
       <c r="K56" t="n">
-        <v>1532.703778356438</v>
+        <v>1370.670658435301</v>
       </c>
       <c r="L56" t="n">
-        <v>1305.113938083618</v>
+        <v>1277.085946776529</v>
       </c>
       <c r="M56" t="n">
-        <v>1452.348289444448</v>
+        <v>1660.981647098361</v>
       </c>
     </row>
     <row r="57">
@@ -3239,25 +3239,25 @@
         <v>136.58</v>
       </c>
       <c r="G57" t="n">
-        <v>-22.32345323055392</v>
+        <v>-63.23095984685051</v>
       </c>
       <c r="H57" t="n">
         <v>1276.18</v>
       </c>
       <c r="I57" t="n">
-        <v>1832.033453230554</v>
+        <v>1872.940959846851</v>
       </c>
       <c r="J57" t="n">
-        <v>1276.305789055147</v>
+        <v>1276.181392062997</v>
       </c>
       <c r="K57" t="n">
-        <v>1628.164817744347</v>
+        <v>1422.481764706734</v>
       </c>
       <c r="L57" t="n">
-        <v>1315.303502383424</v>
+        <v>1277.256464747957</v>
       </c>
       <c r="M57" t="n">
-        <v>1440.569955759633</v>
+        <v>1725.237497431799</v>
       </c>
     </row>
     <row r="58">
@@ -3271,25 +3271,25 @@
         <v>136.48</v>
       </c>
       <c r="G58" t="n">
-        <v>50.56714905195736</v>
+        <v>-2.368177524795328</v>
       </c>
       <c r="H58" t="n">
         <v>1275.79</v>
       </c>
       <c r="I58" t="n">
-        <v>1951.722850948043</v>
+        <v>2004.658177524795</v>
       </c>
       <c r="J58" t="n">
-        <v>1276.0273828745</v>
+        <v>1275.793414551578</v>
       </c>
       <c r="K58" t="n">
-        <v>1749.348099040245</v>
+        <v>1496.731964625065</v>
       </c>
       <c r="L58" t="n">
-        <v>1328.202776873437</v>
+        <v>1277.783291970702</v>
       </c>
       <c r="M58" t="n">
-        <v>1425.333930632157</v>
+        <v>1781.361735852745</v>
       </c>
     </row>
     <row r="59">
@@ -3303,25 +3303,25 @@
         <v>136.38</v>
       </c>
       <c r="G59" t="n">
-        <v>38.07603755878699</v>
+        <v>-12.87609474424789</v>
       </c>
       <c r="H59" t="n">
         <v>1275.28</v>
       </c>
       <c r="I59" t="n">
-        <v>2100.563962441213</v>
+        <v>2151.516094744248</v>
       </c>
       <c r="J59" t="n">
-        <v>1275.719626800375</v>
+        <v>1275.28815360623</v>
       </c>
       <c r="K59" t="n">
-        <v>1898.843141791127</v>
+        <v>1599.375874161651</v>
       </c>
       <c r="L59" t="n">
-        <v>1343.994253056857</v>
+        <v>1278.872982422749</v>
       </c>
       <c r="M59" t="n">
-        <v>1407.724109942574</v>
+        <v>1823.44132406164</v>
       </c>
     </row>
     <row r="60">
@@ -3335,25 +3335,25 @@
         <v>136.28</v>
       </c>
       <c r="G60" t="n">
-        <v>-12.87145145313161</v>
+        <v>-46.65648141980637</v>
       </c>
       <c r="H60" t="n">
         <v>1274.64</v>
       </c>
       <c r="I60" t="n">
-        <v>2281.031451453131</v>
+        <v>2314.816481419806</v>
       </c>
       <c r="J60" t="n">
-        <v>1275.439007476973</v>
+        <v>1274.658954836013</v>
       </c>
       <c r="K60" t="n">
-        <v>2077.786553187206</v>
+        <v>1736.119162710522</v>
       </c>
       <c r="L60" t="n">
-        <v>1362.746881773911</v>
+        <v>1280.943831304452</v>
       </c>
       <c r="M60" t="n">
-        <v>1388.921136209738</v>
+        <v>1846.634939993901</v>
       </c>
     </row>
     <row r="61">
@@ -3367,25 +3367,25 @@
         <v>136.18</v>
       </c>
       <c r="G61" t="n">
-        <v>-12.15191624917497</v>
+        <v>-15.71658824484257</v>
       </c>
       <c r="H61" t="n">
         <v>1273.89</v>
       </c>
       <c r="I61" t="n">
-        <v>2493.061916249175</v>
+        <v>2496.626588244842</v>
       </c>
       <c r="J61" t="n">
-        <v>1275.315118010057</v>
+        <v>1273.932899911647</v>
       </c>
       <c r="K61" t="n">
-        <v>2285.085716991376</v>
+        <v>1911.243073380329</v>
       </c>
       <c r="L61" t="n">
-        <v>1384.307839092661</v>
+        <v>1284.653523063591</v>
       </c>
       <c r="M61" t="n">
-        <v>1370.035240304529</v>
+        <v>1848.106260071336</v>
       </c>
     </row>
     <row r="62">
@@ -3399,25 +3399,25 @@
         <v>136.08</v>
       </c>
       <c r="G62" t="n">
-        <v>31.70336937716274</v>
+        <v>65.93172283812464</v>
       </c>
       <c r="H62" t="n">
         <v>1272.99</v>
       </c>
       <c r="I62" t="n">
-        <v>2733.116630622837</v>
+        <v>2698.888277161876</v>
       </c>
       <c r="J62" t="n">
-        <v>1275.484495111828</v>
+        <v>1273.084529868549</v>
       </c>
       <c r="K62" t="n">
-        <v>2516.626183714561</v>
+        <v>2126.036496826163</v>
       </c>
       <c r="L62" t="n">
-        <v>1408.141826388345</v>
+        <v>1290.872109413807</v>
       </c>
       <c r="M62" t="n">
-        <v>1351.918508771754</v>
+        <v>1827.543633309299</v>
       </c>
     </row>
     <row r="63">
@@ -3431,25 +3431,25 @@
         <v>135.98</v>
       </c>
       <c r="G63" t="n">
-        <v>-29.08939888531768</v>
+        <v>42.5981669588773</v>
       </c>
       <c r="H63" t="n">
         <v>1271.89</v>
       </c>
       <c r="I63" t="n">
-        <v>2993.669398885318</v>
+        <v>2921.981833041123</v>
       </c>
       <c r="J63" t="n">
-        <v>1276.174906177856</v>
+        <v>1272.09279910622</v>
       </c>
       <c r="K63" t="n">
-        <v>2764.821498145023</v>
+        <v>2377.235914832223</v>
       </c>
       <c r="L63" t="n">
-        <v>1433.335302741404</v>
+        <v>1300.789224214895</v>
       </c>
       <c r="M63" t="n">
-        <v>1335.164400963017</v>
+        <v>1787.269503902772</v>
       </c>
     </row>
     <row r="64">
@@ -3463,25 +3463,25 @@
         <v>135.88</v>
       </c>
       <c r="G64" t="n">
-        <v>-58.03414677291994</v>
+        <v>42.21503897417688</v>
       </c>
       <c r="H64" t="n">
         <v>1270.59</v>
       </c>
       <c r="I64" t="n">
-        <v>3263.19414677292</v>
+        <v>3162.944961025823</v>
       </c>
       <c r="J64" t="n">
-        <v>1277.812996390604</v>
+        <v>1271.013596609142</v>
       </c>
       <c r="K64" t="n">
-        <v>3018.561170501622</v>
+        <v>2655.710076362946</v>
       </c>
       <c r="L64" t="n">
-        <v>1458.655186165429</v>
+        <v>1316.006659004556</v>
       </c>
       <c r="M64" t="n">
-        <v>1320.161024218497</v>
+        <v>1731.789833798305</v>
       </c>
     </row>
     <row r="65">
@@ -3495,25 +3495,25 @@
         <v>135.78</v>
       </c>
       <c r="G65" t="n">
-        <v>-85.37233587595529</v>
+        <v>27.46966117612601</v>
       </c>
       <c r="H65" t="n">
         <v>1269.11</v>
       </c>
       <c r="I65" t="n">
-        <v>3526.732335875955</v>
+        <v>3413.890338823874</v>
       </c>
       <c r="J65" t="n">
-        <v>1281.058023917505</v>
+        <v>1269.971449240506</v>
       </c>
       <c r="K65" t="n">
-        <v>3263.628005293375</v>
+        <v>2945.78996095674</v>
       </c>
       <c r="L65" t="n">
-        <v>1482.57891537103</v>
+        <v>1338.489094779957</v>
       </c>
       <c r="M65" t="n">
-        <v>1307.087469063136</v>
+        <v>1666.849878214772</v>
       </c>
     </row>
     <row r="66">
@@ -3527,25 +3527,25 @@
         <v>135.68</v>
       </c>
       <c r="G66" t="n">
-        <v>-105.0031887233636</v>
+        <v>0.7440651699089358</v>
       </c>
       <c r="H66" t="n">
         <v>1267.42</v>
       </c>
       <c r="I66" t="n">
-        <v>3767.183188723363</v>
+        <v>3661.435934830091</v>
       </c>
       <c r="J66" t="n">
-        <v>1286.81348919579</v>
+        <v>1269.125666397691</v>
       </c>
       <c r="K66" t="n">
-        <v>3483.731599353617</v>
+        <v>3225.809641577566</v>
       </c>
       <c r="L66" t="n">
-        <v>1503.353614211124</v>
+        <v>1370.389478138817</v>
       </c>
       <c r="M66" t="n">
-        <v>1295.889870163029</v>
+        <v>1598.323035038897</v>
       </c>
     </row>
     <row r="67">
@@ -3559,25 +3559,25 @@
         <v>135.58</v>
       </c>
       <c r="G67" t="n">
-        <v>-101.2055494593637</v>
+        <v>-21.67022595747994</v>
       </c>
       <c r="H67" t="n">
         <v>1265.55</v>
       </c>
       <c r="I67" t="n">
-        <v>3967.475549459364</v>
+        <v>3887.94022595748</v>
       </c>
       <c r="J67" t="n">
-        <v>1296.436419424834</v>
+        <v>1268.838030154374</v>
       </c>
       <c r="K67" t="n">
-        <v>3662.337255184297</v>
+        <v>3470.404514691078</v>
       </c>
       <c r="L67" t="n">
-        <v>1519.296588125285</v>
+        <v>1413.935334269443</v>
       </c>
       <c r="M67" t="n">
-        <v>1286.444792357167</v>
+        <v>1531.424886478241</v>
       </c>
     </row>
     <row r="68">
@@ -3591,25 +3591,25 @@
         <v>135.48</v>
       </c>
       <c r="G68" t="n">
-        <v>7.686030366867271</v>
+        <v>46.44047846890408</v>
       </c>
       <c r="H68" t="n">
         <v>1263.48</v>
       </c>
       <c r="I68" t="n">
-        <v>4112.963969633132</v>
+        <v>4074.209521531096</v>
       </c>
       <c r="J68" t="n">
-        <v>1311.740498223386</v>
+        <v>1269.650735376152</v>
       </c>
       <c r="K68" t="n">
-        <v>3784.672633257857</v>
+        <v>3654.072441046594</v>
       </c>
       <c r="L68" t="n">
-        <v>1528.910645148288</v>
+        <v>1470.953469002</v>
       </c>
       <c r="M68" t="n">
-        <v>1278.500499266168</v>
+        <v>1470.027802936351</v>
       </c>
     </row>
     <row r="69">
@@ -3623,25 +3623,25 @@
         <v>135.38</v>
       </c>
       <c r="G69" t="n">
-        <v>-50.27130832246803</v>
+        <v>-59.74346637717827</v>
       </c>
       <c r="H69" t="n">
         <v>1261.23</v>
       </c>
       <c r="I69" t="n">
-        <v>4194.031308322468</v>
+        <v>4203.503466377178</v>
       </c>
       <c r="J69" t="n">
-        <v>1335.203802678077</v>
+        <v>1272.503780925539</v>
       </c>
       <c r="K69" t="n">
-        <v>3839.951830950685</v>
+        <v>3755.763488306735</v>
       </c>
       <c r="L69" t="n">
-        <v>1531.191887875555</v>
+        <v>1542.458065798794</v>
       </c>
       <c r="M69" t="n">
-        <v>1271.810237802416</v>
+        <v>1416.542162669627</v>
       </c>
     </row>
     <row r="70">
@@ -3655,25 +3655,25 @@
         <v>135.28</v>
       </c>
       <c r="G70" t="n">
-        <v>26.17951945488312</v>
+        <v>-31.16016923502502</v>
       </c>
       <c r="H70" t="n">
         <v>1258.88</v>
       </c>
       <c r="I70" t="n">
-        <v>4208.100480545117</v>
+        <v>4265.440169235025</v>
       </c>
       <c r="J70" t="n">
-        <v>1370.094517643892</v>
+        <v>1278.929030888606</v>
       </c>
       <c r="K70" t="n">
-        <v>3823.086879304071</v>
+        <v>3763.10091197777</v>
       </c>
       <c r="L70" t="n">
-        <v>1525.811799208783</v>
+        <v>1628.083242572323</v>
       </c>
       <c r="M70" t="n">
-        <v>1266.18491213363</v>
+        <v>1372.034591402011</v>
       </c>
     </row>
     <row r="71">
@@ -3687,25 +3687,25 @@
         <v>135.18</v>
       </c>
       <c r="G71" t="n">
-        <v>156.7046953403933</v>
+        <v>58.73440295478213</v>
       </c>
       <c r="H71" t="n">
         <v>1256.47</v>
       </c>
       <c r="I71" t="n">
-        <v>4160.535304659606</v>
+        <v>4258.505597045218</v>
       </c>
       <c r="J71" t="n">
-        <v>1420.438959325261</v>
+        <v>1291.171831388686</v>
       </c>
       <c r="K71" t="n">
-        <v>3735.4317624291</v>
+        <v>3674.940011932222</v>
       </c>
       <c r="L71" t="n">
-        <v>1513.084260270276</v>
+        <v>1725.420860539588</v>
       </c>
       <c r="M71" t="n">
-        <v>1261.414955039828</v>
+        <v>1336.419426064088</v>
       </c>
     </row>
     <row r="72">
@@ -3719,25 +3719,25 @@
         <v>135.08</v>
       </c>
       <c r="G72" t="n">
-        <v>126.453773940988</v>
+        <v>0.2722048730865936</v>
       </c>
       <c r="H72" t="n">
         <v>1254.01</v>
       </c>
       <c r="I72" t="n">
-        <v>4064.396226059012</v>
+        <v>4190.577795126914</v>
       </c>
       <c r="J72" t="n">
-        <v>1491.026549919445</v>
+        <v>1312.458274725497</v>
       </c>
       <c r="K72" t="n">
-        <v>3584.575752323656</v>
+        <v>3501.637280909368</v>
       </c>
       <c r="L72" t="n">
-        <v>1493.930475973518</v>
+        <v>1829.661882804896</v>
       </c>
       <c r="M72" t="n">
-        <v>1257.292730291559</v>
+        <v>1308.835063532342</v>
       </c>
     </row>
     <row r="73">
@@ -3751,25 +3751,25 @@
         <v>134.98</v>
       </c>
       <c r="G73" t="n">
-        <v>223.7739283950955</v>
+        <v>85.39891059421825</v>
       </c>
       <c r="H73" t="n">
         <v>1251.58</v>
       </c>
       <c r="I73" t="n">
-        <v>3939.056071604904</v>
+        <v>4077.431089405782</v>
       </c>
       <c r="J73" t="n">
-        <v>1587.387958507385</v>
+        <v>1347.355240275107</v>
       </c>
       <c r="K73" t="n">
-        <v>3383.221449765759</v>
+        <v>3262.923719620387</v>
       </c>
       <c r="L73" t="n">
-        <v>1469.833304165851</v>
+        <v>1933.716819130009</v>
       </c>
       <c r="M73" t="n">
-        <v>1253.717531842024</v>
+        <v>1288.093783973114</v>
       </c>
     </row>
     <row r="74">
@@ -3783,25 +3783,25 @@
         <v>134.88</v>
       </c>
       <c r="G74" t="n">
-        <v>67.97040465788314</v>
+        <v>-64.04893144935113</v>
       </c>
       <c r="H74" t="n">
         <v>1249.24</v>
       </c>
       <c r="I74" t="n">
-        <v>3807.689595342117</v>
+        <v>3939.708931449351</v>
       </c>
       <c r="J74" t="n">
-        <v>1715.418475490941</v>
+        <v>1401.881019927432</v>
       </c>
       <c r="K74" t="n">
-        <v>3147.171245885023</v>
+        <v>2983.827802214424</v>
       </c>
       <c r="L74" t="n">
-        <v>1442.536809105378</v>
+        <v>2028.694125855478</v>
       </c>
       <c r="M74" t="n">
-        <v>1250.605392598804</v>
+        <v>1272.871616036764</v>
       </c>
     </row>
     <row r="75">
@@ -3815,25 +3815,25 @@
         <v>134.78</v>
       </c>
       <c r="G75" t="n">
-        <v>47.24269205527162</v>
+        <v>-58.16264014659737</v>
       </c>
       <c r="H75" t="n">
         <v>1247.05</v>
       </c>
       <c r="I75" t="n">
-        <v>3694.387307944728</v>
+        <v>3799.792640146597</v>
       </c>
       <c r="J75" t="n">
-        <v>1880.902909833403</v>
+        <v>1483.569554997711</v>
       </c>
       <c r="K75" t="n">
-        <v>2893.166845129073</v>
+        <v>2690.154902808522</v>
       </c>
       <c r="L75" t="n">
-        <v>1413.838685279076</v>
+        <v>2105.073101290293</v>
       </c>
       <c r="M75" t="n">
-        <v>1247.905696035875</v>
+        <v>1261.919278828364</v>
       </c>
     </row>
     <row r="76">
@@ -3847,25 +3847,25 @@
         <v>134.68</v>
       </c>
       <c r="G76" t="n">
-        <v>47.27450661582361</v>
+        <v>-10.84113492759798</v>
       </c>
       <c r="H76" t="n">
         <v>1245</v>
       </c>
       <c r="I76" t="n">
-        <v>3621.155493384176</v>
+        <v>3679.271134927598</v>
       </c>
       <c r="J76" t="n">
-        <v>2088.715649433504</v>
+        <v>1601.158839411843</v>
       </c>
       <c r="K76" t="n">
-        <v>2636.824065424426</v>
+        <v>2404.509921585661</v>
       </c>
       <c r="L76" t="n">
-        <v>1385.320080444447</v>
+        <v>2154.214193689567</v>
       </c>
       <c r="M76" t="n">
-        <v>1245.526182728735</v>
+        <v>1254.099311736579</v>
       </c>
     </row>
     <row r="77">
@@ -3879,25 +3879,25 @@
         <v>134.58</v>
       </c>
       <c r="G77" t="n">
-        <v>-27.10350670085109</v>
+        <v>-19.23172081690518</v>
       </c>
       <c r="H77" t="n">
         <v>1243.03</v>
       </c>
       <c r="I77" t="n">
-        <v>3605.343506700851</v>
+        <v>3597.471720816905</v>
       </c>
       <c r="J77" t="n">
-        <v>2341.884401866602</v>
+        <v>1763.937867190295</v>
       </c>
       <c r="K77" t="n">
-        <v>2391.164258499113</v>
+        <v>2143.807918361377</v>
       </c>
       <c r="L77" t="n">
-        <v>1358.222958747965</v>
+        <v>2170.03</v>
       </c>
       <c r="M77" t="n">
-        <v>1243.347495313567</v>
+        <v>1248.44724136699</v>
       </c>
     </row>
     <row r="78">
@@ -3911,25 +3911,25 @@
         <v>134.48</v>
       </c>
       <c r="G78" t="n">
-        <v>-70.58858457920724</v>
+        <v>16.44416409429459</v>
       </c>
       <c r="H78" t="n">
         <v>1241.11</v>
       </c>
       <c r="I78" t="n">
-        <v>3657.688584579207</v>
+        <v>3570.655835905705</v>
       </c>
       <c r="J78" t="n">
-        <v>2640.550688668549</v>
+        <v>1980.596625507602</v>
       </c>
       <c r="K78" t="n">
-        <v>2165.857377704097</v>
+        <v>1918.443598309207</v>
       </c>
       <c r="L78" t="n">
-        <v>1333.456423027106</v>
+        <v>2150.324193689557</v>
       </c>
       <c r="M78" t="n">
-        <v>1241.297993317426</v>
+        <v>1244.248335920997</v>
       </c>
     </row>
     <row r="79">
@@ -3943,25 +3943,25 @@
         <v>134.38</v>
       </c>
       <c r="G79" t="n">
-        <v>-148.3368839643067</v>
+        <v>21.55245360222625</v>
       </c>
       <c r="H79" t="n">
         <v>1239.2</v>
       </c>
       <c r="I79" t="n">
-        <v>3780.906883964307</v>
+        <v>3611.017546397774</v>
       </c>
       <c r="J79" t="n">
-        <v>2980.781531154917</v>
+        <v>2257.352686132098</v>
       </c>
       <c r="K79" t="n">
-        <v>1966.975659314375</v>
+        <v>1732.679745836548</v>
       </c>
       <c r="L79" t="n">
-        <v>1311.546900210779</v>
+        <v>2097.223101290275</v>
       </c>
       <c r="M79" t="n">
-        <v>1239.309236076127</v>
+        <v>1240.969494887422</v>
       </c>
     </row>
     <row r="80">
@@ -3975,25 +3975,25 @@
         <v>134.28</v>
       </c>
       <c r="G80" t="n">
-        <v>-247.3023410627843</v>
+        <v>-3.365955898469565</v>
       </c>
       <c r="H80" t="n">
         <v>1237.25</v>
       </c>
       <c r="I80" t="n">
-        <v>3969.052341062784</v>
+        <v>3725.11595589847</v>
       </c>
       <c r="J80" t="n">
-        <v>3353.603816662769</v>
+        <v>2595.622752879568</v>
       </c>
       <c r="K80" t="n">
-        <v>1797.283450021999</v>
+        <v>1585.918330335051</v>
       </c>
       <c r="L80" t="n">
-        <v>1292.676576470523</v>
+        <v>2016.704125855453</v>
       </c>
       <c r="M80" t="n">
-        <v>1237.312289850179</v>
+        <v>1238.22114813813</v>
       </c>
     </row>
     <row r="81">
@@ -4007,25 +4007,25 @@
         <v>134.18</v>
       </c>
       <c r="G81" t="n">
-        <v>-263.3130993663849</v>
+        <v>32.67337104129138</v>
       </c>
       <c r="H81" t="n">
         <v>1235.2</v>
       </c>
       <c r="I81" t="n">
-        <v>4207.673099366385</v>
+        <v>3911.686628958709</v>
       </c>
       <c r="J81" t="n">
-        <v>3744.493883879744</v>
+        <v>2989.534691913414</v>
       </c>
       <c r="K81" t="n">
-        <v>1656.839817183008</v>
+        <v>1474.298193738268</v>
       </c>
       <c r="L81" t="n">
-        <v>1276.750621319015</v>
+        <v>1917.33681912998</v>
       </c>
       <c r="M81" t="n">
-        <v>1235.234857851694</v>
+        <v>1235.718859480412</v>
       </c>
     </row>
     <row r="82">
@@ -4039,25 +4039,25 @@
         <v>134.08</v>
       </c>
       <c r="G82" t="n">
-        <v>-229.8151540673962</v>
+        <v>85.6125010551541</v>
       </c>
       <c r="H82" t="n">
         <v>1232.97</v>
       </c>
       <c r="I82" t="n">
-        <v>4474.845154067396</v>
+        <v>4159.417498944846</v>
       </c>
       <c r="J82" t="n">
-        <v>4133.598776410158</v>
+        <v>3423.863366964075</v>
       </c>
       <c r="K82" t="n">
-        <v>1543.725294549248</v>
+        <v>1392.210668993878</v>
       </c>
       <c r="L82" t="n">
-        <v>1263.465102359108</v>
+        <v>1808.621882804896</v>
       </c>
       <c r="M82" t="n">
-        <v>1232.989143318695</v>
+        <v>1233.239880286888</v>
       </c>
     </row>
     <row r="83">
@@ -4071,25 +4071,25 @@
         <v>133.98</v>
       </c>
       <c r="G83" t="n">
-        <v>-219.3782588401318</v>
+        <v>78.06012811590608</v>
       </c>
       <c r="H83" t="n">
         <v>1230.5</v>
       </c>
       <c r="I83" t="n">
-        <v>4743.208258840132</v>
+        <v>4445.769871884094</v>
       </c>
       <c r="J83" t="n">
-        <v>4496.969378267173</v>
+        <v>3873.238847095994</v>
       </c>
       <c r="K83" t="n">
-        <v>1454.811479233164</v>
+        <v>1333.560103271442</v>
       </c>
       <c r="L83" t="n">
-        <v>1252.421809739813</v>
+        <v>1699.450860539558</v>
       </c>
       <c r="M83" t="n">
-        <v>1230.510317286163</v>
+        <v>1230.636668513243</v>
       </c>
     </row>
     <row r="84">
@@ -4103,25 +4103,25 @@
         <v>133.88</v>
       </c>
       <c r="G84" t="n">
-        <v>-266.2480669372371</v>
+        <v>-21.19433894055692</v>
       </c>
       <c r="H84" t="n">
         <v>1227.8</v>
       </c>
       <c r="I84" t="n">
-        <v>4982.918066937237</v>
+        <v>4737.864338940557</v>
       </c>
       <c r="J84" t="n">
-        <v>4808.81989337462</v>
+        <v>4303.372551348447</v>
       </c>
       <c r="K84" t="n">
-        <v>1386.441670813442</v>
+        <v>1292.646577112587</v>
       </c>
       <c r="L84" t="n">
-        <v>1243.241428144067</v>
+        <v>1597.003242572296</v>
       </c>
       <c r="M84" t="n">
-        <v>1227.805456843488</v>
+        <v>1227.867383300629</v>
       </c>
     </row>
     <row r="85">
@@ -4135,25 +4135,25 @@
         <v>133.78</v>
       </c>
       <c r="G85" t="n">
-        <v>-241.8589474558657</v>
+        <v>-72.65616835827495</v>
       </c>
       <c r="H85" t="n">
         <v>1224.91</v>
       </c>
       <c r="I85" t="n">
-        <v>5165.168947455866</v>
+        <v>4995.966168358275</v>
       </c>
       <c r="J85" t="n">
-        <v>5044.516984484383</v>
+        <v>4674.657438225157</v>
       </c>
       <c r="K85" t="n">
-        <v>1334.87762806938</v>
+        <v>1264.59310951786</v>
       </c>
       <c r="L85" t="n">
-        <v>1235.571223113946</v>
+        <v>1506.138065798772</v>
       </c>
       <c r="M85" t="n">
-        <v>1224.912832302846</v>
+        <v>1224.942346459513</v>
       </c>
     </row>
     <row r="86">
@@ -4167,25 +4167,25 @@
         <v>133.68</v>
       </c>
       <c r="G86" t="n">
-        <v>-142.2463281572072</v>
+        <v>-55.82235400784157</v>
       </c>
       <c r="H86" t="n">
         <v>1221.84</v>
       </c>
       <c r="I86" t="n">
-        <v>5265.876328157207</v>
+        <v>5179.452354007842</v>
       </c>
       <c r="J86" t="n">
-        <v>5183.896258462491</v>
+        <v>4947.984511291234</v>
       </c>
       <c r="K86" t="n">
-        <v>1296.573992905864</v>
+        <v>1245.465191517151</v>
       </c>
       <c r="L86" t="n">
-        <v>1229.056961409479</v>
+        <v>1429.313469001982</v>
       </c>
       <c r="M86" t="n">
-        <v>1221.841442623797</v>
+        <v>1221.855117883674</v>
       </c>
     </row>
     <row r="87">
@@ -4199,25 +4199,25 @@
         <v>133.58</v>
       </c>
       <c r="G87" t="n">
-        <v>-67.35279809639724</v>
+        <v>-52.58374614412514</v>
       </c>
       <c r="H87" t="n">
         <v>1218.63</v>
       </c>
       <c r="I87" t="n">
-        <v>5269.002798096397</v>
+        <v>5254.233746144125</v>
       </c>
       <c r="J87" t="n">
-        <v>5214.373153002078</v>
+        <v>5091.815419524526</v>
       </c>
       <c r="K87" t="n">
-        <v>1268.435701392857</v>
+        <v>1232.316631655463</v>
       </c>
       <c r="L87" t="n">
-        <v>1223.421011776871</v>
+        <v>1367.015334269443</v>
       </c>
       <c r="M87" t="n">
-        <v>1218.630721063839</v>
+        <v>1218.636879236343</v>
       </c>
     </row>
     <row r="88">
@@ -4231,25 +4231,25 @@
         <v>133.48</v>
       </c>
       <c r="G88" t="n">
-        <v>20.18969457897492</v>
+        <v>-10.67494089832599</v>
       </c>
       <c r="H88" t="n">
         <v>1215.36</v>
       </c>
       <c r="I88" t="n">
-        <v>5168.690305421025</v>
+        <v>5199.554940898326</v>
       </c>
       <c r="J88" t="n">
-        <v>5132.980072666029</v>
+        <v>5088.545419524526</v>
       </c>
       <c r="K88" t="n">
-        <v>1247.915924031719</v>
+        <v>1223.07696381459</v>
       </c>
       <c r="L88" t="n">
-        <v>1218.479641066738</v>
+        <v>1318.329478138805</v>
       </c>
       <c r="M88" t="n">
-        <v>1215.360353665585</v>
+        <v>1215.363047661045</v>
       </c>
     </row>
     <row r="89">
@@ -4263,25 +4263,25 @@
         <v>133.38</v>
       </c>
       <c r="G89" t="n">
-        <v>56.31865800405558</v>
+        <v>13.88471385763023</v>
       </c>
       <c r="H89" t="n">
         <v>1212.13</v>
       </c>
       <c r="I89" t="n">
-        <v>4969.751341995944</v>
+        <v>5012.185286142369</v>
       </c>
       <c r="J89" t="n">
-        <v>4946.848512074313</v>
+        <v>4938.274511291234</v>
       </c>
       <c r="K89" t="n">
-        <v>1233.00551063419</v>
+        <v>1216.365284935732</v>
       </c>
       <c r="L89" t="n">
-        <v>1214.122735144201</v>
+        <v>1281.509094779949</v>
       </c>
       <c r="M89" t="n">
-        <v>1212.130170216254</v>
+        <v>1212.131314499027</v>
       </c>
     </row>
     <row r="90">
@@ -4295,25 +4295,25 @@
         <v>133.28</v>
       </c>
       <c r="G90" t="n">
-        <v>32.49754276849853</v>
+        <v>12.21751614279947</v>
       </c>
       <c r="H90" t="n">
         <v>1209.08</v>
       </c>
       <c r="I90" t="n">
-        <v>4686.492457231501</v>
+        <v>4706.7724838572</v>
       </c>
       <c r="J90" t="n">
-        <v>4672.077925153156</v>
+        <v>4658.827438225157</v>
       </c>
       <c r="K90" t="n">
-        <v>1222.212647799601</v>
+        <v>1211.342803845131</v>
       </c>
       <c r="L90" t="n">
-        <v>1210.328853673979</v>
+        <v>1254.49665900455</v>
       </c>
       <c r="M90" t="n">
-        <v>1209.080080387532</v>
+        <v>1209.080551962225</v>
       </c>
     </row>
     <row r="91">
@@ -4327,25 +4327,25 @@
         <v>133.18</v>
       </c>
       <c r="G91" t="n">
-        <v>21.86248957686166</v>
+        <v>49.71978719434719</v>
       </c>
       <c r="H91" t="n">
         <v>1206.3</v>
       </c>
       <c r="I91" t="n">
-        <v>4340.037510423138</v>
+        <v>4312.180212805652</v>
       </c>
       <c r="J91" t="n">
-        <v>4331.133002626723</v>
+        <v>4281.872551348447</v>
       </c>
       <c r="K91" t="n">
-        <v>1214.40617141078</v>
+        <v>1207.476977917817</v>
       </c>
       <c r="L91" t="n">
-        <v>1207.067942360857</v>
+        <v>1235.199224214891</v>
       </c>
       <c r="M91" t="n">
-        <v>1206.300037251681</v>
+        <v>1206.300225632186</v>
       </c>
     </row>
     <row r="92">
@@ -4359,25 +4359,25 @@
         <v>133.08</v>
       </c>
       <c r="G92" t="n">
-        <v>-75.74548941980493</v>
+        <v>13.98727519759223</v>
       </c>
       <c r="H92" t="n">
         <v>1203.88</v>
       </c>
       <c r="I92" t="n">
-        <v>3955.025489419805</v>
+        <v>3865.292724802408</v>
       </c>
       <c r="J92" t="n">
-        <v>3949.625325601821</v>
+        <v>3846.618847095994</v>
       </c>
       <c r="K92" t="n">
-        <v>1208.789733222127</v>
+        <v>1204.476026571642</v>
       </c>
       <c r="L92" t="n">
-        <v>1204.343371538719</v>
+        <v>1221.762109413807</v>
       </c>
       <c r="M92" t="n">
-        <v>1203.880016938014</v>
+        <v>1203.880089788696</v>
       </c>
     </row>
     <row r="93">
@@ -4391,25 +4391,25 @@
         <v>132.98</v>
       </c>
       <c r="G93" t="n">
-        <v>-128.1191770930745</v>
+        <v>24.07879057864557</v>
       </c>
       <c r="H93" t="n">
         <v>1201.85</v>
       </c>
       <c r="I93" t="n">
-        <v>3556.159177093075</v>
+        <v>3403.961209421354</v>
       </c>
       <c r="J93" t="n">
-        <v>3552.943328101049</v>
+        <v>3392.743366964075</v>
       </c>
       <c r="K93" t="n">
-        <v>1204.768104147277</v>
+        <v>1202.143866061078</v>
       </c>
       <c r="L93" t="n">
-        <v>1202.124368625432</v>
+        <v>1212.613523063589</v>
       </c>
       <c r="M93" t="n">
-        <v>1201.850007556635</v>
+        <v>1201.850034782196</v>
       </c>
     </row>
     <row r="94">
@@ -4423,25 +4423,25 @@
         <v>132.88</v>
       </c>
       <c r="G94" t="n">
-        <v>-252.0303543838368</v>
+        <v>-47.7270382405959</v>
       </c>
       <c r="H94" t="n">
         <v>1200.23</v>
       </c>
       <c r="I94" t="n">
-        <v>3165.440354383837</v>
+        <v>2961.137038240596</v>
       </c>
       <c r="J94" t="n">
-        <v>3163.559288052263</v>
+        <v>2954.564691913413</v>
       </c>
       <c r="K94" t="n">
-        <v>1201.932001277524</v>
+        <v>1200.371066503986</v>
       </c>
       <c r="L94" t="n">
-        <v>1200.389425624618</v>
+        <v>1206.533831304451</v>
       </c>
       <c r="M94" t="n">
-        <v>1200.230003307758</v>
+        <v>1200.230013115734</v>
       </c>
     </row>
     <row r="95">
@@ -4455,25 +4455,25 @@
         <v>132.78</v>
       </c>
       <c r="G95" t="n">
-        <v>-328.639454966949</v>
+        <v>-89.49977588189859</v>
       </c>
       <c r="H95" t="n">
         <v>1199</v>
       </c>
       <c r="I95" t="n">
-        <v>2800.269454966949</v>
+        <v>2561.129775881899</v>
       </c>
       <c r="J95" t="n">
-        <v>2799.188278478298</v>
+        <v>2557.372752879568</v>
       </c>
       <c r="K95" t="n">
-        <v>1199.974193166596</v>
+        <v>1199.065930770468</v>
       </c>
       <c r="L95" t="n">
-        <v>1199.090909511073</v>
+        <v>1202.592982422749</v>
       </c>
       <c r="M95" t="n">
-        <v>1199.000001420588</v>
+        <v>1199.000004814086</v>
       </c>
     </row>
     <row r="96">
@@ -4487,25 +4487,25 @@
         <v>132.68</v>
       </c>
       <c r="G96" t="n">
-        <v>-300.5587960871167</v>
+        <v>-46.29920550431871</v>
       </c>
       <c r="H96" t="n">
         <v>1198.09</v>
       </c>
       <c r="I96" t="n">
-        <v>2472.598796087117</v>
+        <v>2218.339205504319</v>
       </c>
       <c r="J96" t="n">
-        <v>2471.98786935721</v>
+        <v>2216.242686132098</v>
       </c>
       <c r="K96" t="n">
-        <v>1198.637219784938</v>
+        <v>1198.12000111405</v>
       </c>
       <c r="L96" t="n">
-        <v>1198.140873621391</v>
+        <v>1200.083291970701</v>
       </c>
       <c r="M96" t="n">
-        <v>1198.09000059858</v>
+        <v>1198.090001719912</v>
       </c>
     </row>
     <row r="97">
@@ -4519,25 +4519,25 @@
         <v>132.58</v>
       </c>
       <c r="G97" t="n">
-        <v>-342.5754088475835</v>
+        <v>-91.58940109608557</v>
       </c>
       <c r="H97" t="n">
         <v>1197.43</v>
       </c>
       <c r="I97" t="n">
-        <v>2189.045408847584</v>
+        <v>1938.059401096086</v>
       </c>
       <c r="J97" t="n">
-        <v>2188.705807708642</v>
+        <v>1936.916625507602</v>
       </c>
       <c r="K97" t="n">
-        <v>1197.731655881945</v>
+        <v>1197.443291188445</v>
       </c>
       <c r="L97" t="n">
-        <v>1197.457938897554</v>
+        <v>1198.506464747957</v>
       </c>
       <c r="M97" t="n">
-        <v>1197.430000247449</v>
+        <v>1197.430000598075</v>
       </c>
     </row>
     <row r="98">
@@ -4551,25 +4551,25 @@
         <v>132.48</v>
       </c>
       <c r="G98" t="n">
-        <v>-299.2334502789599</v>
+        <v>-66.1068093152453</v>
       </c>
       <c r="H98" t="n">
         <v>1196.99</v>
       </c>
       <c r="I98" t="n">
-        <v>1951.63345027896</v>
+        <v>1718.506809315245</v>
       </c>
       <c r="J98" t="n">
-        <v>1951.447575845725</v>
+        <v>1717.897867190295</v>
       </c>
       <c r="K98" t="n">
-        <v>1197.153190158118</v>
+        <v>1196.995732676314</v>
       </c>
       <c r="L98" t="n">
-        <v>1197.005057660886</v>
+        <v>1197.555946776529</v>
       </c>
       <c r="M98" t="n">
-        <v>1196.990000100358</v>
+        <v>1196.990000202417</v>
       </c>
     </row>
     <row r="99">
@@ -4583,25 +4583,25 @@
         <v>132.38</v>
       </c>
       <c r="G99" t="n">
-        <v>-243.3853581007918</v>
+        <v>-37.79636247866074</v>
       </c>
       <c r="H99" t="n">
         <v>1196.68</v>
       </c>
       <c r="I99" t="n">
-        <v>1758.745358100792</v>
+        <v>1553.156362478661</v>
       </c>
       <c r="J99" t="n">
-        <v>1758.645070341018</v>
+        <v>1552.838839411844</v>
       </c>
       <c r="K99" t="n">
-        <v>1196.766637283826</v>
+        <v>1196.682407168591</v>
       </c>
       <c r="L99" t="n">
-        <v>1196.687964041847</v>
+        <v>1196.969681559654</v>
       </c>
       <c r="M99" t="n">
-        <v>1196.680000039931</v>
+        <v>1196.680000066676</v>
       </c>
     </row>
     <row r="100">
@@ -4615,25 +4615,25 @@
         <v>132.28</v>
       </c>
       <c r="G100" t="n">
-        <v>-168.8179518066331</v>
+        <v>4.418230969639581</v>
       </c>
       <c r="H100" t="n">
         <v>1196.45</v>
       </c>
       <c r="I100" t="n">
-        <v>1606.367951806633</v>
+        <v>1433.13176903036</v>
       </c>
       <c r="J100" t="n">
-        <v>1606.314530223961</v>
+        <v>1432.969554997711</v>
       </c>
       <c r="K100" t="n">
-        <v>1196.495137666527</v>
+        <v>1196.450984007032</v>
       </c>
       <c r="L100" t="n">
-        <v>1196.454133631181</v>
+        <v>1196.594360784531</v>
       </c>
       <c r="M100" t="n">
-        <v>1196.450000015586</v>
+        <v>1196.450000021375</v>
       </c>
     </row>
     <row r="101">
@@ -4647,25 +4647,25 @@
         <v>132.18</v>
       </c>
       <c r="G101" t="n">
-        <v>-122.6807370384852</v>
+        <v>17.45766855902275</v>
       </c>
       <c r="H101" t="n">
         <v>1196.29</v>
       </c>
       <c r="I101" t="n">
-        <v>1489.150737038485</v>
+        <v>1349.012331440977</v>
       </c>
       <c r="J101" t="n">
-        <v>1489.122587309475</v>
+        <v>1348.931019927432</v>
       </c>
       <c r="K101" t="n">
-        <v>1196.313077569889</v>
+        <v>1196.29039157848</v>
       </c>
       <c r="L101" t="n">
-        <v>1196.292105450948</v>
+        <v>1196.360043411841</v>
       </c>
       <c r="M101" t="n">
-        <v>1196.290000005968</v>
+        <v>1196.290000006669</v>
       </c>
     </row>
     <row r="102">
@@ -4679,25 +4679,25 @@
         <v>132.08</v>
       </c>
       <c r="G102" t="n">
-        <v>-89.57078141168063</v>
+        <v>19.65469992066255</v>
       </c>
       <c r="H102" t="n">
         <v>1196.17</v>
       </c>
       <c r="I102" t="n">
-        <v>1401.210781411681</v>
+        <v>1291.985300079338</v>
       </c>
       <c r="J102" t="n">
-        <v>1401.196072735646</v>
+        <v>1291.945240275107</v>
       </c>
       <c r="K102" t="n">
-        <v>1196.181578436943</v>
+        <v>1196.170151689023</v>
       </c>
       <c r="L102" t="n">
-        <v>1196.171052363441</v>
+        <v>1196.203088418402</v>
       </c>
       <c r="M102" t="n">
-        <v>1196.170000002242</v>
+        <v>1196.170000002025</v>
       </c>
     </row>
     <row r="103">
@@ -4711,25 +4711,25 @@
         <v>131.98</v>
       </c>
       <c r="G103" t="n">
-        <v>-63.19429997993166</v>
+        <v>19.06228995629567</v>
       </c>
       <c r="H103" t="n">
         <v>1196.1</v>
       </c>
       <c r="I103" t="n">
-        <v>1336.824299979932</v>
+        <v>1254.567710043704</v>
       </c>
       <c r="J103" t="n">
-        <v>1336.816656874504</v>
+        <v>1254.548274725497</v>
       </c>
       <c r="K103" t="n">
-        <v>1196.105700462033</v>
+        <v>1196.100057199171</v>
       </c>
       <c r="L103" t="n">
-        <v>1196.100516160583</v>
+        <v>1196.11521850639</v>
       </c>
       <c r="M103" t="n">
-        <v>1196.100000000826</v>
+        <v>1196.100000000598</v>
       </c>
     </row>
     <row r="104">
@@ -4743,25 +4743,25 @@
         <v>131.88</v>
       </c>
       <c r="G104" t="n">
-        <v>-29.14203841311405</v>
+        <v>30.84886423324951</v>
       </c>
       <c r="H104" t="n">
         <v>1196.04</v>
       </c>
       <c r="I104" t="n">
-        <v>1290.742038413114</v>
+        <v>1230.75113576675</v>
       </c>
       <c r="J104" t="n">
-        <v>1290.738075851973</v>
+        <v>1230.741831388686</v>
       </c>
       <c r="K104" t="n">
-        <v>1196.042753982787</v>
+        <v>1196.040020994763</v>
       </c>
       <c r="L104" t="n">
-        <v>1196.040248423721</v>
+        <v>1196.046814730349</v>
       </c>
       <c r="M104" t="n">
-        <v>1196.040000000299</v>
+        <v>1196.040000000172</v>
       </c>
     </row>
     <row r="105">
@@ -4775,25 +4775,25 @@
         <v>131.78</v>
       </c>
       <c r="G105" t="n">
-        <v>66.94681603792651</v>
+        <v>109.3965648129169</v>
       </c>
       <c r="H105" t="n">
         <v>1195.96</v>
       </c>
       <c r="I105" t="n">
-        <v>1258.463183962074</v>
+        <v>1216.013435187083</v>
       </c>
       <c r="J105" t="n">
-        <v>1258.46112730034</v>
+        <v>1216.009030888606</v>
       </c>
       <c r="K105" t="n">
-        <v>1195.961305550849</v>
+        <v>1195.960007500727</v>
       </c>
       <c r="L105" t="n">
-        <v>1195.960117322344</v>
+        <v>1195.962970959518</v>
       </c>
       <c r="M105" t="n">
-        <v>1195.960000000106</v>
+        <v>1195.960000000048</v>
       </c>
     </row>
     <row r="106">
@@ -4807,25 +4807,25 @@
         <v>131.68</v>
       </c>
       <c r="G106" t="n">
-        <v>56.41579061752736</v>
+        <v>85.60415391338506</v>
       </c>
       <c r="H106" t="n">
         <v>1195.87</v>
       </c>
       <c r="I106" t="n">
-        <v>1236.334209382473</v>
+        <v>1207.145846086615</v>
       </c>
       <c r="J106" t="n">
-        <v>1236.333137370737</v>
+        <v>1207.143780925539</v>
       </c>
       <c r="K106" t="n">
-        <v>1195.870607292429</v>
+        <v>1195.87000260827</v>
       </c>
       <c r="L106" t="n">
-        <v>1195.870054367317</v>
+        <v>1195.871260971052</v>
       </c>
       <c r="M106" t="n">
-        <v>1195.870000000037</v>
+        <v>1195.870000000013</v>
       </c>
     </row>
     <row r="107">
@@ -4839,25 +4839,25 @@
         <v>131.58</v>
       </c>
       <c r="G107" t="n">
-        <v>-55.48948869281617</v>
+        <v>-35.96169596008349</v>
       </c>
       <c r="H107" t="n">
         <v>1195.85</v>
       </c>
       <c r="I107" t="n">
-        <v>1221.549488692816</v>
+        <v>1202.021695960083</v>
       </c>
       <c r="J107" t="n">
-        <v>1221.548926151576</v>
+        <v>1202.020735376152</v>
       </c>
       <c r="K107" t="n">
-        <v>1195.850277180963</v>
+        <v>1195.850000882763</v>
       </c>
       <c r="L107" t="n">
-        <v>1195.850024720344</v>
+        <v>1195.850521028371</v>
       </c>
       <c r="M107" t="n">
-        <v>1195.850000000012</v>
+        <v>1195.850000000003</v>
       </c>
     </row>
     <row r="108">
@@ -4871,25 +4871,25 @@
         <v>131.48</v>
       </c>
       <c r="G108" t="n">
-        <v>-0.4543021944500651</v>
+        <v>12.27152626049292</v>
       </c>
       <c r="H108" t="n">
         <v>1195.85</v>
       </c>
       <c r="I108" t="n">
-        <v>1211.86430219445</v>
+        <v>1199.138473739507</v>
       </c>
       <c r="J108" t="n">
-        <v>1211.864004612144</v>
+        <v>1199.138030154374</v>
       </c>
       <c r="K108" t="n">
-        <v>1195.850124131011</v>
+        <v>1195.85000029078</v>
       </c>
       <c r="L108" t="n">
-        <v>1195.850011028602</v>
+        <v>1195.850209581092</v>
       </c>
       <c r="M108" t="n">
-        <v>1195.850000000004</v>
+        <v>1195.850000000001</v>
       </c>
     </row>
     <row r="109">
@@ -4903,25 +4903,25 @@
         <v>131.38</v>
       </c>
       <c r="G109" t="n">
-        <v>44.81833509536932</v>
+        <v>52.90413021613449</v>
       </c>
       <c r="H109" t="n">
         <v>1195.82</v>
       </c>
       <c r="I109" t="n">
-        <v>1205.611664904631</v>
+        <v>1197.525869783866</v>
       </c>
       <c r="J109" t="n">
-        <v>1205.611506220004</v>
+        <v>1197.525666397691</v>
       </c>
       <c r="K109" t="n">
-        <v>1195.820054542931</v>
+        <v>1195.820000093218</v>
       </c>
       <c r="L109" t="n">
-        <v>1195.820004827538</v>
+        <v>1195.820082066001</v>
       </c>
       <c r="M109" t="n">
-        <v>1195.820000000001</v>
+        <v>1195.82</v>
       </c>
     </row>
     <row r="110">
@@ -4935,22 +4935,22 @@
         <v>131.28</v>
       </c>
       <c r="G110" t="n">
-        <v>12.70516077664638</v>
+        <v>17.71845822809541</v>
       </c>
       <c r="H110" t="n">
         <v>1195.79</v>
       </c>
       <c r="I110" t="n">
-        <v>1201.664839223354</v>
+        <v>1196.651541771904</v>
       </c>
       <c r="J110" t="n">
-        <v>1201.664754047542</v>
+        <v>1196.651449240506</v>
       </c>
       <c r="K110" t="n">
-        <v>1195.790023514078</v>
+        <v>1195.790000029083</v>
       </c>
       <c r="L110" t="n">
-        <v>1195.790002073291</v>
+        <v>1195.790031280991</v>
       </c>
       <c r="M110" t="n">
         <v>1195.79</v>
@@ -4967,22 +4967,22 @@
         <v>131.18</v>
       </c>
       <c r="G111" t="n">
-        <v>48.04104517657561</v>
+        <v>51.07636167343844</v>
       </c>
       <c r="H111" t="n">
         <v>1195.77</v>
       </c>
       <c r="I111" t="n">
-        <v>1199.228954823424</v>
+        <v>1196.193638326562</v>
       </c>
       <c r="J111" t="n">
-        <v>1199.228908919229</v>
+        <v>1196.193596609143</v>
       </c>
       <c r="K111" t="n">
-        <v>1195.770009945781</v>
+        <v>1195.77000000883</v>
       </c>
       <c r="L111" t="n">
-        <v>1195.770000873603</v>
+        <v>1195.770011606178</v>
       </c>
       <c r="M111" t="n">
         <v>1195.77</v>
@@ -4999,22 +4999,22 @@
         <v>131.08</v>
       </c>
       <c r="G112" t="n">
-        <v>-68.28855321761898</v>
+        <v>-66.49281771146161</v>
       </c>
       <c r="H112" t="n">
         <v>1195.77</v>
       </c>
       <c r="I112" t="n">
-        <v>1197.768553217619</v>
+        <v>1195.972817711462</v>
       </c>
       <c r="J112" t="n">
-        <v>1197.768528457254</v>
+        <v>1195.97279910622</v>
       </c>
       <c r="K112" t="n">
-        <v>1195.770004127258</v>
+        <v>1195.770000002609</v>
       </c>
       <c r="L112" t="n">
-        <v>1195.770000361142</v>
+        <v>1195.770004191553</v>
       </c>
       <c r="M112" t="n">
         <v>1195.77</v>
@@ -5031,22 +5031,22 @@
         <v>130.98</v>
       </c>
       <c r="G113" t="n">
-        <v>26.00677547332657</v>
+        <v>27.04546194013233</v>
       </c>
       <c r="H113" t="n">
         <v>1195.79</v>
       </c>
       <c r="I113" t="n">
-        <v>1196.923224526673</v>
+        <v>1195.884538059868</v>
       </c>
       <c r="J113" t="n">
-        <v>1196.923211205136</v>
+        <v>1195.884529868549</v>
       </c>
       <c r="K113" t="n">
-        <v>1195.790001680299</v>
+        <v>1195.79000000075</v>
       </c>
       <c r="L113" t="n">
-        <v>1195.790000146468</v>
+        <v>1195.790001473408</v>
       </c>
       <c r="M113" t="n">
         <v>1195.79</v>
@@ -5063,22 +5063,22 @@
         <v>130.88</v>
       </c>
       <c r="G114" t="n">
-        <v>37.42940706261811</v>
+        <v>38.01709653570492</v>
       </c>
       <c r="H114" t="n">
         <v>1195.76</v>
       </c>
       <c r="I114" t="n">
-        <v>1196.390592937382</v>
+        <v>1195.802903464295</v>
       </c>
       <c r="J114" t="n">
-        <v>1196.390585811565</v>
+        <v>1195.802899911647</v>
       </c>
       <c r="K114" t="n">
-        <v>1195.760000671127</v>
+        <v>1195.76000000021</v>
       </c>
       <c r="L114" t="n">
-        <v>1195.760000058277</v>
+        <v>1195.760000504103</v>
       </c>
       <c r="M114" t="n">
         <v>1195.76</v>
@@ -5095,22 +5095,22 @@
         <v>130.78</v>
       </c>
       <c r="G115" t="n">
-        <v>-0.3443620989482952</v>
+        <v>-0.0189563507785806</v>
       </c>
       <c r="H115" t="n">
         <v>1207.42</v>
       </c>
       <c r="I115" t="n">
-        <v>1207.764362098948</v>
+        <v>1207.438956350779</v>
       </c>
       <c r="J115" t="n">
-        <v>1207.76435832018</v>
+        <v>1207.438954836013</v>
       </c>
       <c r="K115" t="n">
-        <v>1207.42000026297</v>
+        <v>1207.420000000057</v>
       </c>
       <c r="L115" t="n">
-        <v>1207.420000022748</v>
+        <v>1207.420000167861</v>
       </c>
       <c r="M115" t="n">
         <v>1207.42</v>
@@ -5127,22 +5127,22 @@
         <v>130.68</v>
       </c>
       <c r="G116" t="n">
-        <v>-0.1845492636089148</v>
+        <v>-0.008154239997566037</v>
       </c>
       <c r="H116" t="n">
         <v>1171.82</v>
       </c>
       <c r="I116" t="n">
-        <v>1172.004549263609</v>
+        <v>1171.828154239998</v>
       </c>
       <c r="J116" t="n">
-        <v>1172.004547281824</v>
+        <v>1171.82815360623</v>
       </c>
       <c r="K116" t="n">
-        <v>1171.820000101084</v>
+        <v>1171.820000000015</v>
       </c>
       <c r="L116" t="n">
-        <v>1171.820000008711</v>
+        <v>1171.8200000544</v>
       </c>
       <c r="M116" t="n">
         <v>1171.82</v>
@@ -5159,22 +5159,22 @@
         <v>130.58</v>
       </c>
       <c r="G117" t="n">
-        <v>-0.09705894637681922</v>
+        <v>-0.003414811356378777</v>
       </c>
       <c r="H117" t="n">
         <v>1193.28</v>
       </c>
       <c r="I117" t="n">
-        <v>1193.377058946377</v>
+        <v>1193.283414811356</v>
       </c>
       <c r="J117" t="n">
-        <v>1193.37705792046</v>
+        <v>1193.283414551578</v>
       </c>
       <c r="K117" t="n">
-        <v>1193.280000038118</v>
+        <v>1193.280000000004</v>
       </c>
       <c r="L117" t="n">
-        <v>1193.280000003272</v>
+        <v>1193.280000017158</v>
       </c>
       <c r="M117" t="n">
         <v>1193.28</v>
@@ -5191,22 +5191,22 @@
         <v>130.48</v>
       </c>
       <c r="G118" t="n">
-        <v>-0.0500932325624035</v>
+        <v>-0.001392167175481518</v>
       </c>
       <c r="H118" t="n">
         <v>1122.03</v>
       </c>
       <c r="I118" t="n">
-        <v>1122.080093232562</v>
+        <v>1122.031392167175</v>
       </c>
       <c r="J118" t="n">
-        <v>1122.080092709129</v>
+        <v>1122.031392062997</v>
       </c>
       <c r="K118" t="n">
-        <v>1122.0300000141</v>
+        <v>1122.030000000001</v>
       </c>
       <c r="L118" t="n">
-        <v>1122.030000001206</v>
+        <v>1122.030000005266</v>
       </c>
       <c r="M118" t="n">
         <v>1122.03</v>
@@ -5223,22 +5223,22 @@
         <v>130.38</v>
       </c>
       <c r="G119" t="n">
-        <v>-0.0253708763530085</v>
+        <v>-0.000552514544551741</v>
       </c>
       <c r="H119" t="n">
         <v>1224.98</v>
       </c>
       <c r="I119" t="n">
-        <v>1225.005370876353</v>
+        <v>1224.980552514545</v>
       </c>
       <c r="J119" t="n">
-        <v>1225.005370613448</v>
+        <v>1224.980552473716</v>
       </c>
       <c r="K119" t="n">
-        <v>1224.980000005117</v>
+        <v>1224.98</v>
       </c>
       <c r="L119" t="n">
-        <v>1224.980000000436</v>
+        <v>1224.980000001573</v>
       </c>
       <c r="M119" t="n">
         <v>1224.98</v>
@@ -5255,22 +5255,22 @@
         <v>130.28</v>
       </c>
       <c r="G120" t="n">
-        <v>-0.01260946188563139</v>
+        <v>-0.0002134565193046001</v>
       </c>
       <c r="H120" t="n">
         <v>1179.63</v>
       </c>
       <c r="I120" t="n">
-        <v>1179.642609461886</v>
+        <v>1179.630213456519</v>
       </c>
       <c r="J120" t="n">
-        <v>1179.642609332004</v>
+        <v>1179.630213440897</v>
       </c>
       <c r="K120" t="n">
-        <v>1179.630000001821</v>
+        <v>1179.63</v>
       </c>
       <c r="L120" t="n">
-        <v>1179.630000000155</v>
+        <v>1179.630000000457</v>
       </c>
       <c r="M120" t="n">
         <v>1179.63</v>
@@ -5287,22 +5287,22 @@
         <v>130.18</v>
       </c>
       <c r="G121" t="n">
-        <v>-0.006149691921336853</v>
+        <v>-8.027383228181861e-05</v>
       </c>
       <c r="H121" t="n">
         <v>1160.65</v>
       </c>
       <c r="I121" t="n">
-        <v>1160.656149691921</v>
+        <v>1160.650080273832</v>
       </c>
       <c r="J121" t="n">
-        <v>1160.656149628851</v>
+        <v>1160.650080268</v>
       </c>
       <c r="K121" t="n">
-        <v>1160.650000000636</v>
+        <v>1160.65</v>
       </c>
       <c r="L121" t="n">
-        <v>1160.650000000054</v>
+        <v>1160.650000000129</v>
       </c>
       <c r="M121" t="n">
         <v>1160.65</v>
@@ -5319,22 +5319,22 @@
         <v>130.08</v>
       </c>
       <c r="G122" t="n">
-        <v>-0.002943041844218897</v>
+        <v>-2.938480702141533e-05</v>
       </c>
       <c r="H122" t="n">
         <v>1167.95</v>
       </c>
       <c r="I122" t="n">
-        <v>1167.952943041844</v>
+        <v>1167.950029384807</v>
       </c>
       <c r="J122" t="n">
-        <v>1167.952943011755</v>
+        <v>1167.950029382684</v>
       </c>
       <c r="K122" t="n">
-        <v>1167.950000000218</v>
+        <v>1167.95</v>
       </c>
       <c r="L122" t="n">
-        <v>1167.950000000018</v>
+        <v>1167.950000000036</v>
       </c>
       <c r="M122" t="n">
         <v>1167.95</v>
@@ -5351,22 +5351,22 @@
         <v>129.98</v>
       </c>
       <c r="G123" t="n">
-        <v>-0.00138202531729803</v>
+        <v>-1.046987335939775e-05</v>
       </c>
       <c r="H123" t="n">
         <v>1094.96</v>
       </c>
       <c r="I123" t="n">
-        <v>1094.961382025317</v>
+        <v>1094.960010469873</v>
       </c>
       <c r="J123" t="n">
-        <v>1094.961382011219</v>
+        <v>1094.96001046912</v>
       </c>
       <c r="K123" t="n">
-        <v>1094.960000000073</v>
+        <v>1094.96</v>
       </c>
       <c r="L123" t="n">
-        <v>1094.960000000006</v>
+        <v>1094.96000000001</v>
       </c>
       <c r="M123" t="n">
         <v>1094.96</v>
@@ -5383,19 +5383,19 @@
         <v>129.88</v>
       </c>
       <c r="G124" t="n">
-        <v>-0.0006367985367887741</v>
+        <v>-3.630909304774832e-06</v>
       </c>
       <c r="H124" t="n">
         <v>1127.85</v>
       </c>
       <c r="I124" t="n">
-        <v>1127.850636798537</v>
+        <v>1127.850003630909</v>
       </c>
       <c r="J124" t="n">
-        <v>1127.850636792051</v>
+        <v>1127.850003630649</v>
       </c>
       <c r="K124" t="n">
-        <v>1127.850000000024</v>
+        <v>1127.85</v>
       </c>
       <c r="L124" t="n">
         <v>1127.850000000002</v>
@@ -5415,19 +5415,19 @@
         <v>129.78</v>
       </c>
       <c r="G125" t="n">
-        <v>-0.0002879018970816105</v>
+        <v>-1.225548885486205e-06</v>
       </c>
       <c r="H125" t="n">
         <v>1153.15</v>
       </c>
       <c r="I125" t="n">
-        <v>1153.150287901897</v>
+        <v>1153.150001225549</v>
       </c>
       <c r="J125" t="n">
-        <v>1153.150287898968</v>
+        <v>1153.150001225461</v>
       </c>
       <c r="K125" t="n">
-        <v>1153.150000000008</v>
+        <v>1153.15</v>
       </c>
       <c r="L125" t="n">
         <v>1153.150000000001</v>
@@ -5447,19 +5447,19 @@
         <v>129.68</v>
       </c>
       <c r="G126" t="n">
-        <v>-0.0001277124729313073</v>
+        <v>-4.025996531709097e-07</v>
       </c>
       <c r="H126" t="n">
         <v>1176.2</v>
       </c>
       <c r="I126" t="n">
-        <v>1176.200127712473</v>
+        <v>1176.2000004026</v>
       </c>
       <c r="J126" t="n">
-        <v>1176.200127711175</v>
+        <v>1176.200000402571</v>
       </c>
       <c r="K126" t="n">
-        <v>1176.200000000003</v>
+        <v>1176.2</v>
       </c>
       <c r="L126" t="n">
         <v>1176.2</v>
@@ -5479,19 +5479,19 @@
         <v>129.58</v>
       </c>
       <c r="G127" t="n">
-        <v>-5.558509906222753e-05</v>
+        <v>-1.287153281737119e-07</v>
       </c>
       <c r="H127" t="n">
         <v>1085.87</v>
       </c>
       <c r="I127" t="n">
-        <v>1085.870055585099</v>
+        <v>1085.870000128715</v>
       </c>
       <c r="J127" t="n">
-        <v>1085.870055584534</v>
+        <v>1085.870000128706</v>
       </c>
       <c r="K127" t="n">
-        <v>1085.870000000001</v>
+        <v>1085.87</v>
       </c>
       <c r="L127" t="n">
         <v>1085.87</v>
@@ -5511,16 +5511,16 @@
         <v>129.48</v>
       </c>
       <c r="G128" t="n">
-        <v>-2.373612460360164e-05</v>
+        <v>-4.004868969786912e-08</v>
       </c>
       <c r="H128" t="n">
         <v>1142.16</v>
       </c>
       <c r="I128" t="n">
-        <v>1142.160023736125</v>
+        <v>1142.160000040049</v>
       </c>
       <c r="J128" t="n">
-        <v>1142.160023735884</v>
+        <v>1142.160000040046</v>
       </c>
       <c r="K128" t="n">
         <v>1142.16</v>
@@ -5543,16 +5543,16 @@
         <v>129.38</v>
       </c>
       <c r="G129" t="n">
-        <v>-9.944382782123284e-06</v>
+        <v>-1.21265202324139e-08</v>
       </c>
       <c r="H129" t="n">
         <v>1166.26</v>
       </c>
       <c r="I129" t="n">
-        <v>1166.260009944383</v>
+        <v>1166.260000012127</v>
       </c>
       <c r="J129" t="n">
-        <v>1166.260009944282</v>
+        <v>1166.260000012126</v>
       </c>
       <c r="K129" t="n">
         <v>1166.26</v>
@@ -5575,16 +5575,16 @@
         <v>129.28</v>
       </c>
       <c r="G130" t="n">
-        <v>-4.087453817191999e-06</v>
+        <v>-3.573177309590392e-09</v>
       </c>
       <c r="H130" t="n">
         <v>1135.51</v>
       </c>
       <c r="I130" t="n">
-        <v>1135.510004087454</v>
+        <v>1135.510000003573</v>
       </c>
       <c r="J130" t="n">
-        <v>1135.510004087412</v>
+        <v>1135.510000003573</v>
       </c>
       <c r="K130" t="n">
         <v>1135.51</v>
@@ -5607,16 +5607,16 @@
         <v>129.18</v>
       </c>
       <c r="G131" t="n">
-        <v>-1.648259285502718e-06</v>
+        <v>-1.024545781547204e-09</v>
       </c>
       <c r="H131" t="n">
         <v>1121.77</v>
       </c>
       <c r="I131" t="n">
-        <v>1121.770001648259</v>
+        <v>1121.770000001025</v>
       </c>
       <c r="J131" t="n">
-        <v>1121.770001648243</v>
+        <v>1121.770000001025</v>
       </c>
       <c r="K131" t="n">
         <v>1121.77</v>
@@ -5639,16 +5639,16 @@
         <v>129.08</v>
       </c>
       <c r="G132" t="n">
-        <v>-6.520588158309693e-07</v>
+        <v>-2.858087100321427e-10</v>
       </c>
       <c r="H132" t="n">
         <v>1089.89</v>
       </c>
       <c r="I132" t="n">
-        <v>1089.890000652059</v>
+        <v>1089.890000000286</v>
       </c>
       <c r="J132" t="n">
-        <v>1089.890000652052</v>
+        <v>1089.890000000286</v>
       </c>
       <c r="K132" t="n">
         <v>1089.89</v>
@@ -5671,16 +5671,16 @@
         <v>128.98</v>
       </c>
       <c r="G133" t="n">
-        <v>-2.530623532948084e-07</v>
+        <v>-7.753442332614213e-11</v>
       </c>
       <c r="H133" t="n">
         <v>1107.11</v>
       </c>
       <c r="I133" t="n">
-        <v>1107.110000253062</v>
+        <v>1107.110000000077</v>
       </c>
       <c r="J133" t="n">
-        <v>1107.11000025306</v>
+        <v>1107.110000000077</v>
       </c>
       <c r="K133" t="n">
         <v>1107.11</v>
@@ -5703,16 +5703,16 @@
         <v>128.88</v>
       </c>
       <c r="G134" t="n">
-        <v>-9.634732123231515e-08</v>
+        <v>-2.046363078989089e-11</v>
       </c>
       <c r="H134" t="n">
         <v>1103.83</v>
       </c>
       <c r="I134" t="n">
-        <v>1103.830000096347</v>
+        <v>1103.83000000002</v>
       </c>
       <c r="J134" t="n">
-        <v>1103.830000096346</v>
+        <v>1103.83000000002</v>
       </c>
       <c r="K134" t="n">
         <v>1103.83</v>
@@ -5735,16 +5735,16 @@
         <v>128.78</v>
       </c>
       <c r="G135" t="n">
-        <v>-3.598438524932135e-08</v>
+        <v>-5.229594535194337e-12</v>
       </c>
       <c r="H135" t="n">
         <v>1068.4</v>
       </c>
       <c r="I135" t="n">
-        <v>1068.400000035984</v>
+        <v>1068.400000000005</v>
       </c>
       <c r="J135" t="n">
-        <v>1068.400000035984</v>
+        <v>1068.400000000005</v>
       </c>
       <c r="K135" t="n">
         <v>1068.4</v>
@@ -5767,16 +5767,16 @@
         <v>128.68</v>
       </c>
       <c r="G136" t="n">
-        <v>-1.318380782322492e-08</v>
+        <v>-1.364242052659392e-12</v>
       </c>
       <c r="H136" t="n">
         <v>1134.15</v>
       </c>
       <c r="I136" t="n">
-        <v>1134.150000013184</v>
+        <v>1134.150000000001</v>
       </c>
       <c r="J136" t="n">
-        <v>1134.150000013184</v>
+        <v>1134.150000000001</v>
       </c>
       <c r="K136" t="n">
         <v>1134.15</v>
@@ -5799,16 +5799,16 @@
         <v>128.58</v>
       </c>
       <c r="G137" t="n">
-        <v>-4.738240022561513e-09</v>
+        <v>-2.273736754432321e-13</v>
       </c>
       <c r="H137" t="n">
         <v>1072.18</v>
       </c>
       <c r="I137" t="n">
-        <v>1072.180000004738</v>
+        <v>1072.18</v>
       </c>
       <c r="J137" t="n">
-        <v>1072.180000004738</v>
+        <v>1072.18</v>
       </c>
       <c r="K137" t="n">
         <v>1072.18</v>
@@ -5831,16 +5831,16 @@
         <v>128.48</v>
       </c>
       <c r="G138" t="n">
-        <v>-1.670514393481426e-09</v>
+        <v>0</v>
       </c>
       <c r="H138" t="n">
         <v>1133.62</v>
       </c>
       <c r="I138" t="n">
-        <v>1133.62000000167</v>
+        <v>1133.62</v>
       </c>
       <c r="J138" t="n">
-        <v>1133.62000000167</v>
+        <v>1133.62</v>
       </c>
       <c r="K138" t="n">
         <v>1133.62</v>
@@ -5863,16 +5863,16 @@
         <v>128.38</v>
       </c>
       <c r="G139" t="n">
-        <v>-5.777565093012527e-10</v>
+        <v>0</v>
       </c>
       <c r="H139" t="n">
         <v>1117.96</v>
       </c>
       <c r="I139" t="n">
-        <v>1117.960000000578</v>
+        <v>1117.96</v>
       </c>
       <c r="J139" t="n">
-        <v>1117.960000000578</v>
+        <v>1117.96</v>
       </c>
       <c r="K139" t="n">
         <v>1117.96</v>
@@ -5895,16 +5895,16 @@
         <v>128.28</v>
       </c>
       <c r="G140" t="n">
-        <v>-1.95996108232066e-10</v>
+        <v>0</v>
       </c>
       <c r="H140" t="n">
         <v>1074.26</v>
       </c>
       <c r="I140" t="n">
-        <v>1074.260000000196</v>
+        <v>1074.26</v>
       </c>
       <c r="J140" t="n">
-        <v>1074.260000000196</v>
+        <v>1074.26</v>
       </c>
       <c r="K140" t="n">
         <v>1074.26</v>
@@ -5927,16 +5927,16 @@
         <v>128.18</v>
       </c>
       <c r="G141" t="n">
-        <v>-6.52562448522076e-11</v>
+        <v>0</v>
       </c>
       <c r="H141" t="n">
         <v>1140.2</v>
       </c>
       <c r="I141" t="n">
-        <v>1140.200000000065</v>
+        <v>1140.2</v>
       </c>
       <c r="J141" t="n">
-        <v>1140.200000000065</v>
+        <v>1140.2</v>
       </c>
       <c r="K141" t="n">
         <v>1140.2</v>
@@ -5959,16 +5959,16 @@
         <v>128.08</v>
       </c>
       <c r="G142" t="n">
-        <v>-2.137312549166381e-11</v>
+        <v>0</v>
       </c>
       <c r="H142" t="n">
         <v>1069.57</v>
       </c>
       <c r="I142" t="n">
-        <v>1069.570000000021</v>
+        <v>1069.57</v>
       </c>
       <c r="J142" t="n">
-        <v>1069.570000000021</v>
+        <v>1069.57</v>
       </c>
       <c r="K142" t="n">
         <v>1069.57</v>
@@ -5991,16 +5991,16 @@
         <v>127.98</v>
       </c>
       <c r="G143" t="n">
-        <v>-6.821210263296962e-12</v>
+        <v>0</v>
       </c>
       <c r="H143" t="n">
         <v>1084.2</v>
       </c>
       <c r="I143" t="n">
-        <v>1084.200000000007</v>
+        <v>1084.2</v>
       </c>
       <c r="J143" t="n">
-        <v>1084.200000000007</v>
+        <v>1084.2</v>
       </c>
       <c r="K143" t="n">
         <v>1084.2</v>
@@ -6023,16 +6023,16 @@
         <v>127.88</v>
       </c>
       <c r="G144" t="n">
-        <v>-2.046363078989089e-12</v>
+        <v>0</v>
       </c>
       <c r="H144" t="n">
         <v>1073.19</v>
       </c>
       <c r="I144" t="n">
-        <v>1073.190000000002</v>
+        <v>1073.19</v>
       </c>
       <c r="J144" t="n">
-        <v>1073.190000000002</v>
+        <v>1073.19</v>
       </c>
       <c r="K144" t="n">
         <v>1073.19</v>
@@ -6055,16 +6055,16 @@
         <v>127.78</v>
       </c>
       <c r="G145" t="n">
-        <v>-6.821210263296962e-13</v>
+        <v>0</v>
       </c>
       <c r="H145" t="n">
         <v>1042.02</v>
       </c>
       <c r="I145" t="n">
-        <v>1042.020000000001</v>
+        <v>1042.02</v>
       </c>
       <c r="J145" t="n">
-        <v>1042.020000000001</v>
+        <v>1042.02</v>
       </c>
       <c r="K145" t="n">
         <v>1042.02</v>
@@ -6087,7 +6087,7 @@
         <v>127.68</v>
       </c>
       <c r="G146" t="n">
-        <v>-2.273736754432321e-13</v>
+        <v>0</v>
       </c>
       <c r="H146" t="n">
         <v>1090.89</v>

</xml_diff>

<commit_message>
Windows: Optimise Area and Fitting Screen
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/LaSrTiO3.xlsx
+++ b/DATA/UKSAF/LaSrTiO3.xlsx
@@ -405,7 +405,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5581650" cy="4076700"/>
+    <ext cx="5619750" cy="4114800"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -1034,7 +1034,7 @@
       <c r="AF2" s="17" t="inlineStr"/>
       <c r="AG2" s="17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="AH2" s="17" t="inlineStr">
@@ -1116,15 +1116,31 @@
       </c>
       <c r="X3" s="19" t="inlineStr"/>
       <c r="Y3" s="20" t="inlineStr"/>
-      <c r="Z3" s="20" t="inlineStr"/>
+      <c r="Z3" s="20" t="inlineStr">
+        <is>
+          <t>130.53:136.53</t>
+        </is>
+      </c>
       <c r="AA3" s="20" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AB3" s="20" t="inlineStr"/>
-      <c r="AC3" s="20" t="inlineStr"/>
-      <c r="AD3" s="20" t="inlineStr"/>
+      <c r="AB3" s="20" t="inlineStr">
+        <is>
+          <t>0.25:2.25</t>
+        </is>
+      </c>
+      <c r="AC3" s="20" t="inlineStr">
+        <is>
+          <t>0.91:40.91</t>
+        </is>
+      </c>
+      <c r="AD3" s="20" t="inlineStr">
+        <is>
+          <t>1:1E7</t>
+        </is>
+      </c>
       <c r="AE3" s="20" t="inlineStr"/>
       <c r="AF3" s="20" t="inlineStr"/>
       <c r="AG3" s="20" t="inlineStr">
@@ -1212,7 +1228,7 @@
       <c r="AF4" s="17" t="inlineStr"/>
       <c r="AG4" s="17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="AH4" s="17" t="inlineStr">
@@ -1406,7 +1422,7 @@
       <c r="AF6" s="17" t="inlineStr"/>
       <c r="AG6" s="17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="AH6" s="17" t="inlineStr">
@@ -1600,7 +1616,7 @@
       <c r="AF8" s="17" t="inlineStr"/>
       <c r="AG8" s="17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="AH8" s="17" t="inlineStr">

</xml_diff>

<commit_message>
Mac: Add peak labels
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/LaSrTiO3.xlsx
+++ b/DATA/UKSAF/LaSrTiO3.xlsx
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -45,6 +45,10 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="6">
@@ -79,7 +83,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -579,11 +583,29 @@
       <top style="medium"/>
       <bottom style="medium"/>
     </border>
+    <border>
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -681,6 +703,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,7 +829,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5781675" cy="4114800"/>
+    <ext cx="5743575" cy="4076700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -7218,7 +7248,7 @@
 (CPS)</t>
         </is>
       </c>
-      <c r="AP1" s="35" t="inlineStr">
+      <c r="AP1" s="32" t="inlineStr">
         <is>
           <t>Bkg Offset High
 (CPS)</t>
@@ -7303,7 +7333,7 @@
       </c>
       <c r="AG2" s="37" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="AH2" s="37" t="inlineStr">
@@ -7346,7 +7376,7 @@
           <t>0.0</t>
         </is>
       </c>
-      <c r="AP2" s="38" t="inlineStr">
+      <c r="AP2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -7392,7 +7422,7 @@
       </c>
       <c r="AA3" s="40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1:1e7</t>
         </is>
       </c>
       <c r="AB3" s="40" t="inlineStr">
@@ -7417,12 +7447,12 @@
       </c>
       <c r="AF3" s="40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.01:3</t>
         </is>
       </c>
       <c r="AG3" s="40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.01:2</t>
         </is>
       </c>
       <c r="AH3" s="40" t="inlineStr"/>
@@ -7433,7 +7463,6 @@
       <c r="AM3" s="40" t="inlineStr"/>
       <c r="AN3" s="40" t="inlineStr"/>
       <c r="AO3" s="40" t="inlineStr"/>
-      <c r="AP3" s="41" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -7513,7 +7542,7 @@
       </c>
       <c r="AG4" s="37" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="AH4" s="37" t="inlineStr">
@@ -7556,7 +7585,7 @@
           <t>0.0</t>
         </is>
       </c>
-      <c r="AP4" s="38" t="inlineStr">
+      <c r="AP4" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -7602,7 +7631,7 @@
       </c>
       <c r="AA5" s="40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>A*0.5#0.05</t>
         </is>
       </c>
       <c r="AB5" s="40" t="inlineStr">
@@ -7627,12 +7656,12 @@
       </c>
       <c r="AF5" s="40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>A*1</t>
         </is>
       </c>
       <c r="AG5" s="40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>A*1</t>
         </is>
       </c>
       <c r="AH5" s="40" t="inlineStr"/>
@@ -7643,7 +7672,6 @@
       <c r="AM5" s="40" t="inlineStr"/>
       <c r="AN5" s="40" t="inlineStr"/>
       <c r="AO5" s="40" t="inlineStr"/>
-      <c r="AP5" s="41" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -7723,7 +7751,7 @@
       </c>
       <c r="AG6" s="37" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="AH6" s="37" t="inlineStr">
@@ -7766,7 +7794,7 @@
           <t>0.0</t>
         </is>
       </c>
-      <c r="AP6" s="38" t="inlineStr">
+      <c r="AP6" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -7812,7 +7840,7 @@
       </c>
       <c r="AA7" s="40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1:1e7</t>
         </is>
       </c>
       <c r="AB7" s="40" t="inlineStr">
@@ -7837,12 +7865,12 @@
       </c>
       <c r="AF7" s="40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.01:3</t>
         </is>
       </c>
       <c r="AG7" s="40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.01:2</t>
         </is>
       </c>
       <c r="AH7" s="40" t="inlineStr"/>
@@ -7853,7 +7881,6 @@
       <c r="AM7" s="40" t="inlineStr"/>
       <c r="AN7" s="40" t="inlineStr"/>
       <c r="AO7" s="40" t="inlineStr"/>
-      <c r="AP7" s="41" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -7933,7 +7960,7 @@
       </c>
       <c r="AG8" s="37" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="AH8" s="37" t="inlineStr">
@@ -7976,7 +8003,7 @@
           <t>0.0</t>
         </is>
       </c>
-      <c r="AP8" s="38" t="inlineStr">
+      <c r="AP8" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -8022,7 +8049,7 @@
       </c>
       <c r="AA9" s="40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>C*0.5#0.05</t>
         </is>
       </c>
       <c r="AB9" s="40" t="inlineStr">
@@ -8047,12 +8074,12 @@
       </c>
       <c r="AF9" s="40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>C*1</t>
         </is>
       </c>
       <c r="AG9" s="40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>C*1</t>
         </is>
       </c>
       <c r="AH9" s="40" t="inlineStr"/>
@@ -8063,7 +8090,6 @@
       <c r="AM9" s="40" t="inlineStr"/>
       <c r="AN9" s="40" t="inlineStr"/>
       <c r="AO9" s="40" t="inlineStr"/>
-      <c r="AP9" s="41" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -27084,7 +27110,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD5"/>
+  <dimension ref="A1:AE11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27101,11 +27127,11 @@
     <col width="15" customWidth="1" min="7" max="7"/>
     <col width="12" customWidth="1" min="8" max="8"/>
     <col width="6" customWidth="1" min="9" max="9"/>
-    <col width="6" customWidth="1" min="10" max="10"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
     <col width="6" customWidth="1" min="11" max="11"/>
     <col width="8" customWidth="1" min="12" max="12"/>
     <col width="13" customWidth="1" min="13" max="13"/>
-    <col width="25" customWidth="1" min="14" max="14"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
     <col width="23" customWidth="1" min="15" max="15"/>
     <col width="12" customWidth="1" min="16" max="16"/>
     <col width="12" customWidth="1" min="17" max="17"/>
@@ -27122,362 +27148,232 @@
     <col width="17" customWidth="1" min="28" max="28"/>
     <col width="14" customWidth="1" min="29" max="29"/>
     <col width="14" customWidth="1" min="30" max="30"/>
+    <col width="6" customWidth="1" min="31" max="31"/>
   </cols>
   <sheetData>
     <row r="1"/>
     <row r="2">
-      <c r="B2" s="42" t="inlineStr">
+      <c r="B2" s="49" t="inlineStr">
+        <is>
+          <t>Sample 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="50" t="inlineStr">
         <is>
           <t>Peak
 Label</t>
         </is>
       </c>
-      <c r="C2" s="42" t="inlineStr">
+      <c r="C3" s="51" t="inlineStr">
         <is>
           <t>Position
 (eV)</t>
         </is>
       </c>
-      <c r="D2" s="42" t="inlineStr">
+      <c r="D3" s="51" t="inlineStr">
         <is>
           <t>Height
 (CPS)</t>
         </is>
       </c>
-      <c r="E2" s="42" t="inlineStr">
+      <c r="E3" s="51" t="inlineStr">
         <is>
           <t>FWHM
 (eV)</t>
         </is>
       </c>
-      <c r="F2" s="42" t="inlineStr">
+      <c r="F3" s="51" t="inlineStr">
         <is>
           <t>L/G 
 σ/γ (%)</t>
         </is>
       </c>
-      <c r="G2" s="42" t="inlineStr">
+      <c r="G3" s="51" t="inlineStr">
         <is>
           <t>Area
 (CPS.eV)</t>
         </is>
       </c>
-      <c r="H2" s="42" t="inlineStr">
+      <c r="H3" s="51" t="inlineStr">
         <is>
           <t>Atomic
 (%)</t>
         </is>
       </c>
-      <c r="I2" s="42" t="inlineStr">
+      <c r="I3" s="51" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="J2" s="42" t="inlineStr">
+      <c r="J3" s="51" t="inlineStr">
         <is>
           <t>RSF</t>
         </is>
       </c>
-      <c r="K2" s="42" t="inlineStr">
+      <c r="K3" s="51" t="inlineStr">
         <is>
           <t>TXFN</t>
         </is>
       </c>
-      <c r="L2" s="42" t="inlineStr">
+      <c r="L3" s="51" t="inlineStr">
         <is>
           <t>ECF</t>
         </is>
       </c>
-      <c r="M2" s="42" t="inlineStr">
+      <c r="M3" s="51" t="inlineStr">
         <is>
           <t>Instr.</t>
         </is>
       </c>
-      <c r="N2" s="42" t="inlineStr">
+      <c r="N3" s="51" t="inlineStr">
         <is>
           <t>Fitting Model</t>
         </is>
       </c>
-      <c r="O2" s="42" t="inlineStr">
+      <c r="O3" s="51" t="inlineStr">
         <is>
           <t>Corr. Area
  Ac (a.u.)</t>
         </is>
       </c>
-      <c r="P2" s="42" t="inlineStr">
+      <c r="P3" s="51" t="inlineStr">
         <is>
           <t>σ or α
 W_g</t>
         </is>
       </c>
-      <c r="Q2" s="42" t="inlineStr">
+      <c r="Q3" s="51" t="inlineStr">
         <is>
           <t>γ or β
 W_l</t>
         </is>
       </c>
-      <c r="R2" s="42" t="inlineStr">
+      <c r="R3" s="51" t="inlineStr">
         <is>
           <t>Bkg Type</t>
         </is>
       </c>
-      <c r="S2" s="42" t="inlineStr">
+      <c r="S3" s="51" t="inlineStr">
         <is>
           <t>Bkg Low
 (eV)</t>
         </is>
       </c>
-      <c r="T2" s="42" t="inlineStr">
+      <c r="T3" s="51" t="inlineStr">
         <is>
           <t>Bkg High
 (eV)</t>
         </is>
       </c>
-      <c r="U2" s="42" t="inlineStr">
+      <c r="U3" s="51" t="inlineStr">
         <is>
           <t>Bkg Offset Low
 (CPS)</t>
         </is>
       </c>
-      <c r="V2" s="42" t="inlineStr">
+      <c r="V3" s="51" t="inlineStr">
         <is>
           <t>Bkg Offset High
 (CPS)</t>
         </is>
       </c>
-      <c r="W2" s="42" t="inlineStr">
+      <c r="W3" s="51" t="inlineStr">
         <is>
           <t>Sheetname</t>
         </is>
       </c>
-      <c r="X2" s="42" t="inlineStr">
+      <c r="X3" s="51" t="inlineStr">
         <is>
           <t>Position
 Constraint</t>
         </is>
       </c>
-      <c r="Y2" s="42" t="inlineStr">
+      <c r="Y3" s="51" t="inlineStr">
         <is>
           <t>Height
 Constraint</t>
         </is>
       </c>
-      <c r="Z2" s="42" t="inlineStr">
+      <c r="Z3" s="51" t="inlineStr">
         <is>
           <t>FWHM
 Constraint</t>
         </is>
       </c>
-      <c r="AA2" s="42" t="inlineStr">
+      <c r="AA3" s="51" t="inlineStr">
         <is>
           <t>L/G
 Constraint</t>
         </is>
       </c>
-      <c r="AB2" s="42" t="inlineStr">
+      <c r="AB3" s="51" t="inlineStr">
         <is>
           <t>Area
 Constraint</t>
         </is>
       </c>
-      <c r="AC2" s="42" t="inlineStr">
+      <c r="AC3" s="51" t="inlineStr">
         <is>
           <t>σ
 Constraint</t>
         </is>
       </c>
-      <c r="AD2" s="42" t="inlineStr">
+      <c r="AD3" s="51" t="inlineStr">
         <is>
           <t>γ
 Constraint</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="43" t="inlineStr">
-        <is>
-          <t>Sr3d5/2 p1</t>
-        </is>
-      </c>
-      <c r="C3" s="44" t="inlineStr">
-        <is>
-          <t>133.44</t>
-        </is>
-      </c>
-      <c r="D3" s="44" t="inlineStr">
-        <is>
-          <t>3515.41</t>
-        </is>
-      </c>
-      <c r="E3" s="44" t="inlineStr">
-        <is>
-          <t>1.07</t>
-        </is>
-      </c>
-      <c r="F3" s="44" t="inlineStr">
-        <is>
-          <t>28.0</t>
-        </is>
-      </c>
-      <c r="G3" s="44" t="inlineStr">
-        <is>
-          <t>4634.68</t>
-        </is>
-      </c>
-      <c r="H3" s="44" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="I3" s="44" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J3" s="44" t="inlineStr">
-        <is>
-          <t>4.25</t>
-        </is>
-      </c>
-      <c r="K3" s="44" t="inlineStr">
-        <is>
-          <t>1.00</t>
-        </is>
-      </c>
-      <c r="L3" s="44" t="inlineStr">
-        <is>
-          <t>TPP-2M</t>
-        </is>
-      </c>
-      <c r="M3" s="44" t="inlineStr">
-        <is>
-          <t>A-ALTHERMO1</t>
-        </is>
-      </c>
-      <c r="N3" s="44" t="inlineStr">
-        <is>
-          <t>Voigt (Area, L/G, σ, S)</t>
-        </is>
-      </c>
-      <c r="O3" s="44" t="inlineStr">
-        <is>
-          <t>13.94</t>
-        </is>
-      </c>
-      <c r="P3" s="44" t="inlineStr">
-        <is>
-          <t>0.89</t>
-        </is>
-      </c>
-      <c r="Q3" s="44" t="inlineStr">
-        <is>
-          <t>0.35</t>
-        </is>
-      </c>
-      <c r="R3" s="44" t="inlineStr"/>
-      <c r="S3" s="44" t="inlineStr">
-        <is>
-          <t>126.08</t>
-        </is>
-      </c>
-      <c r="T3" s="44" t="inlineStr">
-        <is>
-          <t>142.08</t>
-        </is>
-      </c>
-      <c r="U3" s="44" t="inlineStr"/>
-      <c r="V3" s="44" t="inlineStr"/>
-      <c r="W3" s="44" t="inlineStr">
-        <is>
-          <t>Sr3d</t>
-        </is>
-      </c>
-      <c r="X3" s="44" t="inlineStr">
-        <is>
-          <t>126.08,142.08</t>
-        </is>
-      </c>
-      <c r="Y3" s="44" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Z3" s="44" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AA3" s="44" t="inlineStr">
-        <is>
-          <t>15:85</t>
-        </is>
-      </c>
-      <c r="AB3" s="44" t="inlineStr">
-        <is>
-          <t>1:1e7</t>
-        </is>
-      </c>
-      <c r="AC3" s="44" t="inlineStr">
-        <is>
-          <t>0.2:1.5</t>
-        </is>
-      </c>
-      <c r="AD3" s="45" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="AE3" s="52" t="n"/>
     </row>
     <row r="4">
       <c r="B4" s="43" t="inlineStr">
         <is>
-          <t>Sr3d3/2 p2</t>
+          <t>Sr3d5/2 p1</t>
         </is>
       </c>
       <c r="C4" s="44" t="inlineStr">
         <is>
-          <t>135.19</t>
+          <t>133.51</t>
         </is>
       </c>
       <c r="D4" s="44" t="inlineStr">
         <is>
-          <t>2465.25</t>
+          <t>3828.02</t>
         </is>
       </c>
       <c r="E4" s="44" t="inlineStr">
         <is>
-          <t>1.07</t>
+          <t>1.23</t>
         </is>
       </c>
       <c r="F4" s="44" t="inlineStr">
         <is>
-          <t>28.0</t>
+          <t>16.51</t>
         </is>
       </c>
       <c r="G4" s="44" t="inlineStr">
         <is>
-          <t>3250.16</t>
+          <t>5012.00</t>
         </is>
       </c>
       <c r="H4" s="44" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>21.78</t>
         </is>
       </c>
       <c r="I4" s="44" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J4" s="44" t="inlineStr">
-        <is>
-          <t>2.93</t>
-        </is>
-      </c>
-      <c r="K4" s="44" t="inlineStr">
-        <is>
-          <t>1.00</t>
-        </is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="J4" s="44" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="K4" s="44" t="n">
+        <v>1</v>
       </c>
       <c r="L4" s="44" t="inlineStr">
         <is>
@@ -27491,34 +27387,30 @@
       </c>
       <c r="N4" s="44" t="inlineStr">
         <is>
-          <t>Voigt (Area, L/G, σ, S)</t>
+          <t>GL (Area)</t>
         </is>
       </c>
       <c r="O4" s="44" t="inlineStr">
         <is>
-          <t>14.20</t>
+          <t>15.07</t>
         </is>
       </c>
       <c r="P4" s="44" t="inlineStr">
         <is>
-          <t>0.89</t>
+          <t>1.23</t>
         </is>
       </c>
       <c r="Q4" s="44" t="inlineStr">
         <is>
-          <t>0.35</t>
+          <t>0.17</t>
         </is>
       </c>
       <c r="R4" s="44" t="inlineStr"/>
-      <c r="S4" s="44" t="inlineStr">
-        <is>
-          <t>126.08</t>
-        </is>
-      </c>
-      <c r="T4" s="44" t="inlineStr">
-        <is>
-          <t>142.08</t>
-        </is>
+      <c r="S4" s="44" t="n">
+        <v>126.08</v>
+      </c>
+      <c r="T4" s="44" t="n">
+        <v>142.08</v>
       </c>
       <c r="U4" s="44" t="inlineStr"/>
       <c r="V4" s="44" t="inlineStr"/>
@@ -27529,174 +27421,920 @@
       </c>
       <c r="X4" s="44" t="inlineStr">
         <is>
+          <t>126.08,142.08</t>
+        </is>
+      </c>
+      <c r="Y4" s="44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z4" s="44" t="inlineStr">
+        <is>
+          <t>0.3:3.5</t>
+        </is>
+      </c>
+      <c r="AA4" s="44" t="inlineStr">
+        <is>
+          <t>2:80</t>
+        </is>
+      </c>
+      <c r="AB4" s="44" t="inlineStr">
+        <is>
+          <t>1:1e7</t>
+        </is>
+      </c>
+      <c r="AC4" s="44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD4" s="44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE4" s="38" t="n"/>
+    </row>
+    <row r="5">
+      <c r="B5" s="43" t="inlineStr">
+        <is>
+          <t>Sr3d3/2 p2</t>
+        </is>
+      </c>
+      <c r="C5" s="44" t="inlineStr">
+        <is>
+          <t>135.31</t>
+        </is>
+      </c>
+      <c r="D5" s="44" t="inlineStr">
+        <is>
+          <t>2625.08</t>
+        </is>
+      </c>
+      <c r="E5" s="44" t="inlineStr">
+        <is>
+          <t>1.23</t>
+        </is>
+      </c>
+      <c r="F5" s="44" t="inlineStr">
+        <is>
+          <t>16.51</t>
+        </is>
+      </c>
+      <c r="G5" s="44" t="inlineStr">
+        <is>
+          <t>3437.00</t>
+        </is>
+      </c>
+      <c r="H5" s="44" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I5" s="44" t="inlineStr"/>
+      <c r="J5" s="44" t="n">
+        <v>2.927432</v>
+      </c>
+      <c r="K5" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="44" t="inlineStr">
+        <is>
+          <t>TPP-2M</t>
+        </is>
+      </c>
+      <c r="M5" s="44" t="inlineStr">
+        <is>
+          <t>A-ALTHERMO1</t>
+        </is>
+      </c>
+      <c r="N5" s="44" t="inlineStr">
+        <is>
+          <t>GL (Area)</t>
+        </is>
+      </c>
+      <c r="O5" s="44" t="inlineStr">
+        <is>
+          <t>15.02</t>
+        </is>
+      </c>
+      <c r="P5" s="44" t="inlineStr">
+        <is>
+          <t>2.90</t>
+        </is>
+      </c>
+      <c r="Q5" s="44" t="inlineStr">
+        <is>
+          <t>0.34</t>
+        </is>
+      </c>
+      <c r="R5" s="44" t="inlineStr"/>
+      <c r="S5" s="44" t="n">
+        <v>126.08</v>
+      </c>
+      <c r="T5" s="44" t="n">
+        <v>142.08</v>
+      </c>
+      <c r="U5" s="44" t="inlineStr"/>
+      <c r="V5" s="44" t="inlineStr"/>
+      <c r="W5" s="44" t="inlineStr">
+        <is>
+          <t>Sr3d</t>
+        </is>
+      </c>
+      <c r="X5" s="44" t="inlineStr">
+        <is>
           <t>A+1.7#0.2</t>
         </is>
       </c>
-      <c r="Y4" s="44" t="inlineStr">
+      <c r="Y5" s="44" t="inlineStr">
+        <is>
+          <t>A*0.667#0.05</t>
+        </is>
+      </c>
+      <c r="Z5" s="44" t="inlineStr">
+        <is>
+          <t>A*1</t>
+        </is>
+      </c>
+      <c r="AA5" s="44" t="inlineStr">
+        <is>
+          <t>A*1</t>
+        </is>
+      </c>
+      <c r="AB5" s="44" t="inlineStr">
+        <is>
+          <t>A*0.667#0.05</t>
+        </is>
+      </c>
+      <c r="AC5" s="44" t="inlineStr">
+        <is>
+          <t>A*1</t>
+        </is>
+      </c>
+      <c r="AD5" s="44" t="inlineStr">
+        <is>
+          <t>A*1</t>
+        </is>
+      </c>
+      <c r="AE5" s="38" t="n"/>
+    </row>
+    <row r="6">
+      <c r="B6" s="43" t="inlineStr">
+        <is>
+          <t>Sr3d5/2 p3</t>
+        </is>
+      </c>
+      <c r="C6" s="44" t="inlineStr">
+        <is>
+          <t>134.47</t>
+        </is>
+      </c>
+      <c r="D6" s="44" t="inlineStr">
+        <is>
+          <t>1010.47</t>
+        </is>
+      </c>
+      <c r="E6" s="44" t="inlineStr">
+        <is>
+          <t>1.23</t>
+        </is>
+      </c>
+      <c r="F6" s="44" t="inlineStr">
+        <is>
+          <t>16.51</t>
+        </is>
+      </c>
+      <c r="G6" s="44" t="inlineStr">
+        <is>
+          <t>1323.00</t>
+        </is>
+      </c>
+      <c r="H6" s="44" t="inlineStr">
+        <is>
+          <t>5.75</t>
+        </is>
+      </c>
+      <c r="I6" s="44" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="J6" s="44" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="K6" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="44" t="inlineStr">
+        <is>
+          <t>TPP-2M</t>
+        </is>
+      </c>
+      <c r="M6" s="44" t="inlineStr">
+        <is>
+          <t>A-ALTHERMO1</t>
+        </is>
+      </c>
+      <c r="N6" s="44" t="inlineStr">
+        <is>
+          <t>GL (Area)</t>
+        </is>
+      </c>
+      <c r="O6" s="44" t="inlineStr">
+        <is>
+          <t>3.98</t>
+        </is>
+      </c>
+      <c r="P6" s="44" t="inlineStr">
+        <is>
+          <t>6.83</t>
+        </is>
+      </c>
+      <c r="Q6" s="44" t="inlineStr">
+        <is>
+          <t>0.68</t>
+        </is>
+      </c>
+      <c r="R6" s="44" t="inlineStr"/>
+      <c r="S6" s="44" t="n">
+        <v>126.08</v>
+      </c>
+      <c r="T6" s="44" t="n">
+        <v>142.08</v>
+      </c>
+      <c r="U6" s="44" t="inlineStr"/>
+      <c r="V6" s="44" t="inlineStr"/>
+      <c r="W6" s="44" t="inlineStr">
+        <is>
+          <t>Sr3d</t>
+        </is>
+      </c>
+      <c r="X6" s="44" t="inlineStr">
+        <is>
+          <t>A+1.05#0.1</t>
+        </is>
+      </c>
+      <c r="Y6" s="44" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="Z4" s="44" t="inlineStr">
+      <c r="Z6" s="44" t="inlineStr">
+        <is>
+          <t>A*1</t>
+        </is>
+      </c>
+      <c r="AA6" s="44" t="inlineStr">
+        <is>
+          <t>A*1</t>
+        </is>
+      </c>
+      <c r="AB6" s="44" t="inlineStr">
+        <is>
+          <t>1:1e7</t>
+        </is>
+      </c>
+      <c r="AC6" s="44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD6" s="44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE6" s="38" t="n"/>
+    </row>
+    <row r="7">
+      <c r="B7" s="43" t="inlineStr">
+        <is>
+          <t>Sr3d3/2 p4</t>
+        </is>
+      </c>
+      <c r="C7" s="44" t="inlineStr">
+        <is>
+          <t>136.23</t>
+        </is>
+      </c>
+      <c r="D7" s="44" t="inlineStr">
+        <is>
+          <t>623.46</t>
+        </is>
+      </c>
+      <c r="E7" s="44" t="inlineStr">
+        <is>
+          <t>1.23</t>
+        </is>
+      </c>
+      <c r="F7" s="44" t="inlineStr">
+        <is>
+          <t>16.51</t>
+        </is>
+      </c>
+      <c r="G7" s="44" t="inlineStr">
+        <is>
+          <t>816.29</t>
+        </is>
+      </c>
+      <c r="H7" s="44" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I7" s="44" t="inlineStr"/>
+      <c r="J7" s="44" t="n">
+        <v>2.927432</v>
+      </c>
+      <c r="K7" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="44" t="inlineStr">
+        <is>
+          <t>TPP-2M</t>
+        </is>
+      </c>
+      <c r="M7" s="44" t="inlineStr">
+        <is>
+          <t>A-ALTHERMO1</t>
+        </is>
+      </c>
+      <c r="N7" s="44" t="inlineStr">
+        <is>
+          <t>GL (Area)</t>
+        </is>
+      </c>
+      <c r="O7" s="44" t="inlineStr">
+        <is>
+          <t>3.57</t>
+        </is>
+      </c>
+      <c r="P7" s="44" t="inlineStr">
+        <is>
+          <t>16.08</t>
+        </is>
+      </c>
+      <c r="Q7" s="44" t="inlineStr">
+        <is>
+          <t>1.36</t>
+        </is>
+      </c>
+      <c r="R7" s="44" t="inlineStr"/>
+      <c r="S7" s="44" t="n">
+        <v>126.08</v>
+      </c>
+      <c r="T7" s="44" t="n">
+        <v>142.08</v>
+      </c>
+      <c r="U7" s="44" t="inlineStr"/>
+      <c r="V7" s="44" t="inlineStr"/>
+      <c r="W7" s="44" t="inlineStr">
+        <is>
+          <t>Sr3d</t>
+        </is>
+      </c>
+      <c r="X7" s="44" t="inlineStr">
+        <is>
+          <t>C+1.7#0.2</t>
+        </is>
+      </c>
+      <c r="Y7" s="44" t="inlineStr">
+        <is>
+          <t>C*0.667#0.05</t>
+        </is>
+      </c>
+      <c r="Z7" s="44" t="inlineStr">
+        <is>
+          <t>C*1</t>
+        </is>
+      </c>
+      <c r="AA7" s="44" t="inlineStr">
+        <is>
+          <t>C*1</t>
+        </is>
+      </c>
+      <c r="AB7" s="44" t="inlineStr">
+        <is>
+          <t>C*0.667#0.05</t>
+        </is>
+      </c>
+      <c r="AC7" s="44" t="inlineStr">
+        <is>
+          <t>C*1</t>
+        </is>
+      </c>
+      <c r="AD7" s="44" t="inlineStr">
+        <is>
+          <t>C*1</t>
+        </is>
+      </c>
+      <c r="AE7" s="38" t="n"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="43" t="inlineStr">
+        <is>
+          <t>Ti2p3/2 p1</t>
+        </is>
+      </c>
+      <c r="C8" s="44" t="inlineStr">
+        <is>
+          <t>458.99</t>
+        </is>
+      </c>
+      <c r="D8" s="44" t="inlineStr">
+        <is>
+          <t>7303.71</t>
+        </is>
+      </c>
+      <c r="E8" s="44" t="inlineStr">
+        <is>
+          <t>1.42</t>
+        </is>
+      </c>
+      <c r="F8" s="44" t="inlineStr">
+        <is>
+          <t>35.82</t>
+        </is>
+      </c>
+      <c r="G8" s="44" t="inlineStr">
+        <is>
+          <t>13115.00</t>
+        </is>
+      </c>
+      <c r="H8" s="44" t="inlineStr">
+        <is>
+          <t>67.70</t>
+        </is>
+      </c>
+      <c r="I8" s="44" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="J8" s="44" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="K8" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="44" t="inlineStr">
+        <is>
+          <t>TPP-2M</t>
+        </is>
+      </c>
+      <c r="M8" s="44" t="inlineStr">
+        <is>
+          <t>A-ALTHERMO1</t>
+        </is>
+      </c>
+      <c r="N8" s="44" t="inlineStr">
+        <is>
+          <t>Voigt (Area, L/G, σ)</t>
+        </is>
+      </c>
+      <c r="O8" s="44" t="inlineStr">
+        <is>
+          <t>46.90</t>
+        </is>
+      </c>
+      <c r="P8" s="44" t="inlineStr">
+        <is>
+          <t>1.07</t>
+        </is>
+      </c>
+      <c r="Q8" s="44" t="inlineStr">
+        <is>
+          <t>0.60</t>
+        </is>
+      </c>
+      <c r="R8" s="44" t="inlineStr"/>
+      <c r="S8" s="44" t="n">
+        <v>448.08</v>
+      </c>
+      <c r="T8" s="44" t="n">
+        <v>475.08</v>
+      </c>
+      <c r="U8" s="44" t="inlineStr"/>
+      <c r="V8" s="44" t="inlineStr"/>
+      <c r="W8" s="44" t="inlineStr">
+        <is>
+          <t>Ti2p</t>
+        </is>
+      </c>
+      <c r="X8" s="44" t="inlineStr">
+        <is>
+          <t>448.08,475.08</t>
+        </is>
+      </c>
+      <c r="Y8" s="44" t="inlineStr">
+        <is>
+          <t>1:1e7</t>
+        </is>
+      </c>
+      <c r="Z8" s="44" t="inlineStr">
         <is>
           <t>0.3:3.5</t>
         </is>
       </c>
-      <c r="AA4" s="44" t="inlineStr">
+      <c r="AA8" s="44" t="inlineStr">
+        <is>
+          <t>1:80</t>
+        </is>
+      </c>
+      <c r="AB8" s="44" t="inlineStr">
+        <is>
+          <t>1:1e7</t>
+        </is>
+      </c>
+      <c r="AC8" s="44" t="inlineStr">
+        <is>
+          <t>0.01:3</t>
+        </is>
+      </c>
+      <c r="AD8" s="44" t="inlineStr">
+        <is>
+          <t>0.01:3</t>
+        </is>
+      </c>
+      <c r="AE8" s="38" t="n"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="43" t="inlineStr">
+        <is>
+          <t>Ti2p1/2 p2</t>
+        </is>
+      </c>
+      <c r="C9" s="44" t="inlineStr">
+        <is>
+          <t>464.71</t>
+        </is>
+      </c>
+      <c r="D9" s="44" t="inlineStr">
+        <is>
+          <t>2263.63</t>
+        </is>
+      </c>
+      <c r="E9" s="44" t="inlineStr">
+        <is>
+          <t>2.21</t>
+        </is>
+      </c>
+      <c r="F9" s="44" t="inlineStr">
+        <is>
+          <t>35.82</t>
+        </is>
+      </c>
+      <c r="G9" s="44" t="inlineStr">
+        <is>
+          <t>6306.00</t>
+        </is>
+      </c>
+      <c r="H9" s="44" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I9" s="44" t="inlineStr"/>
+      <c r="J9" s="44" t="n">
+        <v>2.055385</v>
+      </c>
+      <c r="K9" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="44" t="inlineStr">
+        <is>
+          <t>TPP-2M</t>
+        </is>
+      </c>
+      <c r="M9" s="44" t="inlineStr">
+        <is>
+          <t>A-ALTHERMO1</t>
+        </is>
+      </c>
+      <c r="N9" s="44" t="inlineStr">
+        <is>
+          <t>Voigt (Area, L/G, σ)</t>
+        </is>
+      </c>
+      <c r="O9" s="44" t="inlineStr">
+        <is>
+          <t>48.64</t>
+        </is>
+      </c>
+      <c r="P9" s="44" t="inlineStr">
+        <is>
+          <t>1.66</t>
+        </is>
+      </c>
+      <c r="Q9" s="44" t="inlineStr">
+        <is>
+          <t>0.93</t>
+        </is>
+      </c>
+      <c r="R9" s="44" t="inlineStr"/>
+      <c r="S9" s="44" t="n">
+        <v>448.08</v>
+      </c>
+      <c r="T9" s="44" t="n">
+        <v>475.08</v>
+      </c>
+      <c r="U9" s="44" t="inlineStr"/>
+      <c r="V9" s="44" t="inlineStr"/>
+      <c r="W9" s="44" t="inlineStr">
+        <is>
+          <t>Ti2p</t>
+        </is>
+      </c>
+      <c r="X9" s="44" t="inlineStr">
+        <is>
+          <t>A+5.7#0.2</t>
+        </is>
+      </c>
+      <c r="Y9" s="44" t="inlineStr">
+        <is>
+          <t>A*0.5#0.05</t>
+        </is>
+      </c>
+      <c r="Z9" s="44" t="inlineStr">
         <is>
           <t>A*1</t>
         </is>
       </c>
-      <c r="AB4" s="44" t="inlineStr">
-        <is>
-          <t>A*0.667#0.05</t>
-        </is>
-      </c>
-      <c r="AC4" s="44" t="inlineStr">
+      <c r="AA9" s="44" t="inlineStr">
         <is>
           <t>A*1</t>
         </is>
       </c>
-      <c r="AD4" s="45" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="46" t="inlineStr">
-        <is>
-          <t>Sr3d5/2 p3</t>
-        </is>
-      </c>
-      <c r="C5" s="47" t="inlineStr">
-        <is>
-          <t>134.17</t>
-        </is>
-      </c>
-      <c r="D5" s="47" t="inlineStr">
-        <is>
-          <t>1394.46</t>
-        </is>
-      </c>
-      <c r="E5" s="47" t="inlineStr">
+      <c r="AB9" s="44" t="inlineStr">
+        <is>
+          <t>A*0.5#0.05</t>
+        </is>
+      </c>
+      <c r="AC9" s="44" t="inlineStr">
+        <is>
+          <t>0.01:3</t>
+        </is>
+      </c>
+      <c r="AD9" s="44" t="inlineStr">
+        <is>
+          <t>A*1</t>
+        </is>
+      </c>
+      <c r="AE9" s="38" t="n"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="43" t="inlineStr">
+        <is>
+          <t>Ti2p3/2 p3</t>
+        </is>
+      </c>
+      <c r="C10" s="44" t="inlineStr">
+        <is>
+          <t>456.86</t>
+        </is>
+      </c>
+      <c r="D10" s="44" t="inlineStr">
+        <is>
+          <t>514.57</t>
+        </is>
+      </c>
+      <c r="E10" s="44" t="inlineStr">
+        <is>
+          <t>1.42</t>
+        </is>
+      </c>
+      <c r="F10" s="44" t="inlineStr">
+        <is>
+          <t>35.82</t>
+        </is>
+      </c>
+      <c r="G10" s="44" t="inlineStr">
+        <is>
+          <t>924.00</t>
+        </is>
+      </c>
+      <c r="H10" s="44" t="inlineStr">
+        <is>
+          <t>4.76</t>
+        </is>
+      </c>
+      <c r="I10" s="44" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="J10" s="44" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="K10" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" s="44" t="inlineStr">
+        <is>
+          <t>TPP-2M</t>
+        </is>
+      </c>
+      <c r="M10" s="44" t="inlineStr">
+        <is>
+          <t>A-ALTHERMO1</t>
+        </is>
+      </c>
+      <c r="N10" s="44" t="inlineStr">
+        <is>
+          <t>Voigt (Area, L/G, σ)</t>
+        </is>
+      </c>
+      <c r="O10" s="44" t="inlineStr">
+        <is>
+          <t>3.30</t>
+        </is>
+      </c>
+      <c r="P10" s="44" t="inlineStr">
         <is>
           <t>1.07</t>
         </is>
       </c>
-      <c r="F5" s="47" t="inlineStr">
-        <is>
-          <t>28.0</t>
-        </is>
-      </c>
-      <c r="G5" s="47" t="inlineStr">
-        <is>
-          <t>1838.44</t>
-        </is>
-      </c>
-      <c r="H5" s="47" t="inlineStr">
+      <c r="Q10" s="44" t="inlineStr">
+        <is>
+          <t>0.60</t>
+        </is>
+      </c>
+      <c r="R10" s="44" t="inlineStr"/>
+      <c r="S10" s="44" t="n">
+        <v>448.08</v>
+      </c>
+      <c r="T10" s="44" t="n">
+        <v>475.08</v>
+      </c>
+      <c r="U10" s="44" t="inlineStr"/>
+      <c r="V10" s="44" t="inlineStr"/>
+      <c r="W10" s="44" t="inlineStr">
+        <is>
+          <t>Ti2p</t>
+        </is>
+      </c>
+      <c r="X10" s="44" t="inlineStr">
+        <is>
+          <t>448.08,475.08</t>
+        </is>
+      </c>
+      <c r="Y10" s="44" t="inlineStr">
+        <is>
+          <t>1:1e7</t>
+        </is>
+      </c>
+      <c r="Z10" s="44" t="inlineStr">
+        <is>
+          <t>0.3:3.5</t>
+        </is>
+      </c>
+      <c r="AA10" s="44" t="inlineStr">
+        <is>
+          <t>A*1</t>
+        </is>
+      </c>
+      <c r="AB10" s="44" t="inlineStr">
+        <is>
+          <t>1:1e7</t>
+        </is>
+      </c>
+      <c r="AC10" s="44" t="inlineStr">
+        <is>
+          <t>A*1</t>
+        </is>
+      </c>
+      <c r="AD10" s="44" t="inlineStr">
+        <is>
+          <t>0.01:3</t>
+        </is>
+      </c>
+      <c r="AE10" s="38" t="n"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="46" t="inlineStr">
+        <is>
+          <t>Ti2p1/2 p4</t>
+        </is>
+      </c>
+      <c r="C11" s="47" t="inlineStr">
+        <is>
+          <t>462.76</t>
+        </is>
+      </c>
+      <c r="D11" s="47" t="inlineStr">
+        <is>
+          <t>182.44</t>
+        </is>
+      </c>
+      <c r="E11" s="47" t="inlineStr">
+        <is>
+          <t>2.21</t>
+        </is>
+      </c>
+      <c r="F11" s="47" t="inlineStr">
+        <is>
+          <t>35.82</t>
+        </is>
+      </c>
+      <c r="G11" s="47" t="inlineStr">
+        <is>
+          <t>508.20</t>
+        </is>
+      </c>
+      <c r="H11" s="47" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="I5" s="47" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J5" s="47" t="inlineStr">
-        <is>
-          <t>4.25</t>
-        </is>
-      </c>
-      <c r="K5" s="47" t="inlineStr">
-        <is>
-          <t>1.00</t>
-        </is>
-      </c>
-      <c r="L5" s="47" t="inlineStr">
+      <c r="I11" s="47" t="inlineStr"/>
+      <c r="J11" s="47" t="n">
+        <v>2.055385</v>
+      </c>
+      <c r="K11" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="47" t="inlineStr">
         <is>
           <t>TPP-2M</t>
         </is>
       </c>
-      <c r="M5" s="47" t="inlineStr">
+      <c r="M11" s="47" t="inlineStr">
         <is>
           <t>A-ALTHERMO1</t>
         </is>
       </c>
-      <c r="N5" s="47" t="inlineStr">
-        <is>
-          <t>Voigt (Area, L/G, σ, S)</t>
-        </is>
-      </c>
-      <c r="O5" s="47" t="inlineStr">
-        <is>
-          <t>5.53</t>
-        </is>
-      </c>
-      <c r="P5" s="47" t="inlineStr">
-        <is>
-          <t>0.89</t>
-        </is>
-      </c>
-      <c r="Q5" s="47" t="inlineStr">
-        <is>
-          <t>0.35</t>
-        </is>
-      </c>
-      <c r="R5" s="47" t="inlineStr"/>
-      <c r="S5" s="47" t="inlineStr">
-        <is>
-          <t>126.08</t>
-        </is>
-      </c>
-      <c r="T5" s="47" t="inlineStr">
-        <is>
-          <t>142.08</t>
-        </is>
-      </c>
-      <c r="U5" s="47" t="inlineStr"/>
-      <c r="V5" s="47" t="inlineStr"/>
-      <c r="W5" s="47" t="inlineStr">
-        <is>
-          <t>Sr3d</t>
-        </is>
-      </c>
-      <c r="X5" s="47" t="inlineStr">
-        <is>
-          <t>126.08,142.08</t>
-        </is>
-      </c>
-      <c r="Y5" s="47" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Z5" s="47" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AA5" s="47" t="inlineStr">
-        <is>
-          <t>A*1</t>
-        </is>
-      </c>
-      <c r="AB5" s="47" t="inlineStr">
-        <is>
-          <t>1:1e7</t>
-        </is>
-      </c>
-      <c r="AC5" s="47" t="inlineStr">
-        <is>
-          <t>A*1</t>
-        </is>
-      </c>
-      <c r="AD5" s="48" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="N11" s="47" t="inlineStr">
+        <is>
+          <t>Voigt (Area, L/G, σ)</t>
+        </is>
+      </c>
+      <c r="O11" s="47" t="inlineStr">
+        <is>
+          <t>3.91</t>
+        </is>
+      </c>
+      <c r="P11" s="47" t="inlineStr">
+        <is>
+          <t>1.66</t>
+        </is>
+      </c>
+      <c r="Q11" s="47" t="inlineStr">
+        <is>
+          <t>0.93</t>
+        </is>
+      </c>
+      <c r="R11" s="47" t="inlineStr"/>
+      <c r="S11" s="47" t="n">
+        <v>448.08</v>
+      </c>
+      <c r="T11" s="47" t="n">
+        <v>475.08</v>
+      </c>
+      <c r="U11" s="47" t="inlineStr"/>
+      <c r="V11" s="47" t="inlineStr"/>
+      <c r="W11" s="47" t="inlineStr">
+        <is>
+          <t>Ti2p</t>
+        </is>
+      </c>
+      <c r="X11" s="47" t="inlineStr">
+        <is>
+          <t>C+5.7#0.2</t>
+        </is>
+      </c>
+      <c r="Y11" s="47" t="inlineStr">
+        <is>
+          <t>C*0.5#0.05</t>
+        </is>
+      </c>
+      <c r="Z11" s="47" t="inlineStr">
+        <is>
+          <t>C*1</t>
+        </is>
+      </c>
+      <c r="AA11" s="47" t="inlineStr">
+        <is>
+          <t>C*1</t>
+        </is>
+      </c>
+      <c r="AB11" s="47" t="inlineStr">
+        <is>
+          <t>C*0.5#0.05</t>
+        </is>
+      </c>
+      <c r="AC11" s="47" t="inlineStr">
+        <is>
+          <t>B*1</t>
+        </is>
+      </c>
+      <c r="AD11" s="47" t="inlineStr">
+        <is>
+          <t>C*1</t>
+        </is>
+      </c>
+      <c r="AE11" s="41" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Mac: Improve .SPE for multiprobe 2
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/LaSrTiO3.xlsx
+++ b/DATA/UKSAF/LaSrTiO3.xlsx
@@ -11,6 +11,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="O1s" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="C1s" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results Table" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sr3d1" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -605,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -711,6 +712,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -27110,7 +27114,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE11"/>
+  <dimension ref="B2:AE11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27151,7 +27155,6 @@
     <col width="6" customWidth="1" min="31" max="31"/>
   </cols>
   <sheetData>
-    <row r="1"/>
     <row r="2">
       <c r="B2" s="49" t="inlineStr">
         <is>
@@ -28335,6 +28338,2301 @@
         </is>
       </c>
       <c r="AE11" s="41" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D162"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="53" t="inlineStr">
+        <is>
+          <t>BE</t>
+        </is>
+      </c>
+      <c r="B1" s="53" t="inlineStr">
+        <is>
+          <t>Raw Data</t>
+        </is>
+      </c>
+      <c r="C1" s="53" t="inlineStr">
+        <is>
+          <t>Background</t>
+        </is>
+      </c>
+      <c r="D1" s="53" t="inlineStr">
+        <is>
+          <t>Transmission</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>142.08</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1321.18</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1321.18</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>141.98</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1369.78</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1369.78</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>141.88</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1356.16</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1356.16</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>141.78</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1341.5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1341.5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>141.68</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1332.29</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1332.29</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>141.58</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1338.15</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1338.15</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>141.48</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1335.29</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1335.29</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>141.38</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1341.58</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1341.58</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>141.28</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1349.18</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1349.18</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>141.18</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1344.67</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1344.67</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>141.08</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1336.42</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1336.42</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>140.98</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1281.16</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1281.16</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>140.88</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1323.55</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1323.55</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>140.78</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1322.81</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1322.81</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>140.68</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1352.14</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1352.14</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>140.58</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1304.84</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1304.84</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>140.48</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1296.85</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1296.85</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>140.38</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1297.71</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1297.71</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>140.28</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1346.66</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1346.66</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>140.18</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1293.78</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1293.78</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>140.08</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1294.58</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1294.58</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>139.98</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1282.76</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1282.76</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>139.88</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1291.45</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1291.45</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>139.78</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1275.21</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1275.21</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>139.68</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1311.33</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1311.33</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>139.58</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1287.86</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1287.86</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>139.48</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1305.54</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1305.54</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>139.38</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1286.85</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1286.85</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>139.28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1284.54</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1284.54</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>139.18</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1296.58</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1296.58</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>139.08</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1288.78</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1288.78</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>138.98</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1262.37</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1262.37</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>138.88</v>
+      </c>
+      <c r="B34" t="n">
+        <v>1298.36</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1298.36</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>138.78</v>
+      </c>
+      <c r="B35" t="n">
+        <v>1231.15</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1261.45</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>138.68</v>
+      </c>
+      <c r="B36" t="n">
+        <v>1288.75</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1261.03</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>138.58</v>
+      </c>
+      <c r="B37" t="n">
+        <v>1264.45</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1261.03</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>138.48</v>
+      </c>
+      <c r="B38" t="n">
+        <v>1303.52</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1261.01</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>138.38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>1312.96</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1260.99</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>138.28</v>
+      </c>
+      <c r="B40" t="n">
+        <v>1276.13</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1260.96</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>138.18</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1283.01</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1260.93</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>138.08</v>
+      </c>
+      <c r="B42" t="n">
+        <v>1251.47</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1260.91</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>137.98</v>
+      </c>
+      <c r="B43" t="n">
+        <v>1268.26</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1260.91</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>137.88</v>
+      </c>
+      <c r="B44" t="n">
+        <v>1314.52</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1260.91</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>137.78</v>
+      </c>
+      <c r="B45" t="n">
+        <v>1314.35</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1260.89</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>137.68</v>
+      </c>
+      <c r="B46" t="n">
+        <v>1361.59</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1260.84</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>137.58</v>
+      </c>
+      <c r="B47" t="n">
+        <v>1319.42</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1260.78</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>137.48</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1305.06</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1260.71</v>
+      </c>
+      <c r="D48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>137.38</v>
+      </c>
+      <c r="B49" t="n">
+        <v>1395.15</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1260.67</v>
+      </c>
+      <c r="D49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>137.28</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1382.15</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1260.6</v>
+      </c>
+      <c r="D50" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>137.18</v>
+      </c>
+      <c r="B51" t="n">
+        <v>1422.48</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1260.5</v>
+      </c>
+      <c r="D51" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>137.08</v>
+      </c>
+      <c r="B52" t="n">
+        <v>1462.63</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1260.38</v>
+      </c>
+      <c r="D52" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>136.98</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1526.56</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1260.23</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>136.88</v>
+      </c>
+      <c r="B54" t="n">
+        <v>1601.68</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1260.04</v>
+      </c>
+      <c r="D54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>136.78</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1650.31</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1259.79</v>
+      </c>
+      <c r="D55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>136.68</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1734.49</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1259.49</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>136.58</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1809.71</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1259.14</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>136.48</v>
+      </c>
+      <c r="B58" t="n">
+        <v>2002.29</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1258.72</v>
+      </c>
+      <c r="D58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>136.38</v>
+      </c>
+      <c r="B59" t="n">
+        <v>2138.64</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1258.18</v>
+      </c>
+      <c r="D59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>136.28</v>
+      </c>
+      <c r="B60" t="n">
+        <v>2268.16</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1257.51</v>
+      </c>
+      <c r="D60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>136.18</v>
+      </c>
+      <c r="B61" t="n">
+        <v>2480.91</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1256.73</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>136.08</v>
+      </c>
+      <c r="B62" t="n">
+        <v>2764.82</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1255.8</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>135.98</v>
+      </c>
+      <c r="B63" t="n">
+        <v>2964.58</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1254.66</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>135.88</v>
+      </c>
+      <c r="B64" t="n">
+        <v>3205.16</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1253.32</v>
+      </c>
+      <c r="D64" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>135.78</v>
+      </c>
+      <c r="B65" t="n">
+        <v>3441.36</v>
+      </c>
+      <c r="C65" t="n">
+        <v>1251.78</v>
+      </c>
+      <c r="D65" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>135.68</v>
+      </c>
+      <c r="B66" t="n">
+        <v>3662.18</v>
+      </c>
+      <c r="C66" t="n">
+        <v>1250.05</v>
+      </c>
+      <c r="D66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>135.58</v>
+      </c>
+      <c r="B67" t="n">
+        <v>3866.27</v>
+      </c>
+      <c r="C67" t="n">
+        <v>1248.11</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>135.48</v>
+      </c>
+      <c r="B68" t="n">
+        <v>4120.65</v>
+      </c>
+      <c r="C68" t="n">
+        <v>1245.98</v>
+      </c>
+      <c r="D68" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>135.38</v>
+      </c>
+      <c r="B69" t="n">
+        <v>4143.76</v>
+      </c>
+      <c r="C69" t="n">
+        <v>1243.67</v>
+      </c>
+      <c r="D69" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>135.28</v>
+      </c>
+      <c r="B70" t="n">
+        <v>4234.28</v>
+      </c>
+      <c r="C70" t="n">
+        <v>1241.25</v>
+      </c>
+      <c r="D70" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>135.18</v>
+      </c>
+      <c r="B71" t="n">
+        <v>4317.24</v>
+      </c>
+      <c r="C71" t="n">
+        <v>1238.77</v>
+      </c>
+      <c r="D71" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>135.08</v>
+      </c>
+      <c r="B72" t="n">
+        <v>4190.85</v>
+      </c>
+      <c r="C72" t="n">
+        <v>1236.24</v>
+      </c>
+      <c r="D72" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>134.98</v>
+      </c>
+      <c r="B73" t="n">
+        <v>4162.83</v>
+      </c>
+      <c r="C73" t="n">
+        <v>1233.74</v>
+      </c>
+      <c r="D73" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>134.88</v>
+      </c>
+      <c r="B74" t="n">
+        <v>3875.66</v>
+      </c>
+      <c r="C74" t="n">
+        <v>1231.33</v>
+      </c>
+      <c r="D74" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>134.78</v>
+      </c>
+      <c r="B75" t="n">
+        <v>3741.63</v>
+      </c>
+      <c r="C75" t="n">
+        <v>1229.07</v>
+      </c>
+      <c r="D75" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>134.68</v>
+      </c>
+      <c r="B76" t="n">
+        <v>3668.43</v>
+      </c>
+      <c r="C76" t="n">
+        <v>1226.96</v>
+      </c>
+      <c r="D76" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>134.58</v>
+      </c>
+      <c r="B77" t="n">
+        <v>3578.24</v>
+      </c>
+      <c r="C77" t="n">
+        <v>1224.93</v>
+      </c>
+      <c r="D77" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>134.48</v>
+      </c>
+      <c r="B78" t="n">
+        <v>3587.1</v>
+      </c>
+      <c r="C78" t="n">
+        <v>1222.96</v>
+      </c>
+      <c r="D78" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>134.38</v>
+      </c>
+      <c r="B79" t="n">
+        <v>3632.57</v>
+      </c>
+      <c r="C79" t="n">
+        <v>1220.99</v>
+      </c>
+      <c r="D79" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>134.28</v>
+      </c>
+      <c r="B80" t="n">
+        <v>3721.75</v>
+      </c>
+      <c r="C80" t="n">
+        <v>1218.98</v>
+      </c>
+      <c r="D80" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>134.18</v>
+      </c>
+      <c r="B81" t="n">
+        <v>3944.36</v>
+      </c>
+      <c r="C81" t="n">
+        <v>1216.87</v>
+      </c>
+      <c r="D81" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>134.08</v>
+      </c>
+      <c r="B82" t="n">
+        <v>4245.03</v>
+      </c>
+      <c r="C82" t="n">
+        <v>1214.57</v>
+      </c>
+      <c r="D82" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>133.98</v>
+      </c>
+      <c r="B83" t="n">
+        <v>4523.83</v>
+      </c>
+      <c r="C83" t="n">
+        <v>1212.03</v>
+      </c>
+      <c r="D83" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>133.88</v>
+      </c>
+      <c r="B84" t="n">
+        <v>4716.67</v>
+      </c>
+      <c r="C84" t="n">
+        <v>1209.26</v>
+      </c>
+      <c r="D84" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>133.78</v>
+      </c>
+      <c r="B85" t="n">
+        <v>4923.31</v>
+      </c>
+      <c r="C85" t="n">
+        <v>1206.29</v>
+      </c>
+      <c r="D85" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>133.68</v>
+      </c>
+      <c r="B86" t="n">
+        <v>5123.63</v>
+      </c>
+      <c r="C86" t="n">
+        <v>1203.14</v>
+      </c>
+      <c r="D86" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>133.58</v>
+      </c>
+      <c r="B87" t="n">
+        <v>5201.65</v>
+      </c>
+      <c r="C87" t="n">
+        <v>1199.84</v>
+      </c>
+      <c r="D87" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>133.48</v>
+      </c>
+      <c r="B88" t="n">
+        <v>5188.88</v>
+      </c>
+      <c r="C88" t="n">
+        <v>1196.47</v>
+      </c>
+      <c r="D88" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>133.38</v>
+      </c>
+      <c r="B89" t="n">
+        <v>5026.07</v>
+      </c>
+      <c r="C89" t="n">
+        <v>1193.16</v>
+      </c>
+      <c r="D89" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>133.28</v>
+      </c>
+      <c r="B90" t="n">
+        <v>4718.99</v>
+      </c>
+      <c r="C90" t="n">
+        <v>1190.02</v>
+      </c>
+      <c r="D90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>133.18</v>
+      </c>
+      <c r="B91" t="n">
+        <v>4361.9</v>
+      </c>
+      <c r="C91" t="n">
+        <v>1187.17</v>
+      </c>
+      <c r="D91" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>133.08</v>
+      </c>
+      <c r="B92" t="n">
+        <v>3879.28</v>
+      </c>
+      <c r="C92" t="n">
+        <v>1184.67</v>
+      </c>
+      <c r="D92" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>132.98</v>
+      </c>
+      <c r="B93" t="n">
+        <v>3428.04</v>
+      </c>
+      <c r="C93" t="n">
+        <v>1182.58</v>
+      </c>
+      <c r="D93" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>132.88</v>
+      </c>
+      <c r="B94" t="n">
+        <v>2913.41</v>
+      </c>
+      <c r="C94" t="n">
+        <v>1180.9</v>
+      </c>
+      <c r="D94" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>132.78</v>
+      </c>
+      <c r="B95" t="n">
+        <v>2471.63</v>
+      </c>
+      <c r="C95" t="n">
+        <v>1179.63</v>
+      </c>
+      <c r="D95" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>132.68</v>
+      </c>
+      <c r="B96" t="n">
+        <v>2172.04</v>
+      </c>
+      <c r="C96" t="n">
+        <v>1178.68</v>
+      </c>
+      <c r="D96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>132.58</v>
+      </c>
+      <c r="B97" t="n">
+        <v>1846.47</v>
+      </c>
+      <c r="C97" t="n">
+        <v>1177.99</v>
+      </c>
+      <c r="D97" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>132.48</v>
+      </c>
+      <c r="B98" t="n">
+        <v>1652.4</v>
+      </c>
+      <c r="C98" t="n">
+        <v>1177.52</v>
+      </c>
+      <c r="D98" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>132.38</v>
+      </c>
+      <c r="B99" t="n">
+        <v>1515.36</v>
+      </c>
+      <c r="C99" t="n">
+        <v>1177.19</v>
+      </c>
+      <c r="D99" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>132.28</v>
+      </c>
+      <c r="B100" t="n">
+        <v>1437.55</v>
+      </c>
+      <c r="C100" t="n">
+        <v>1176.94</v>
+      </c>
+      <c r="D100" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>132.18</v>
+      </c>
+      <c r="B101" t="n">
+        <v>1366.47</v>
+      </c>
+      <c r="C101" t="n">
+        <v>1176.76</v>
+      </c>
+      <c r="D101" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>132.08</v>
+      </c>
+      <c r="B102" t="n">
+        <v>1311.64</v>
+      </c>
+      <c r="C102" t="n">
+        <v>1176.62</v>
+      </c>
+      <c r="D102" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>131.98</v>
+      </c>
+      <c r="B103" t="n">
+        <v>1273.63</v>
+      </c>
+      <c r="C103" t="n">
+        <v>1176.53</v>
+      </c>
+      <c r="D103" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>131.88</v>
+      </c>
+      <c r="B104" t="n">
+        <v>1261.6</v>
+      </c>
+      <c r="C104" t="n">
+        <v>1176.45</v>
+      </c>
+      <c r="D104" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>131.78</v>
+      </c>
+      <c r="B105" t="n">
+        <v>1325.41</v>
+      </c>
+      <c r="C105" t="n">
+        <v>1176.36</v>
+      </c>
+      <c r="D105" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>131.68</v>
+      </c>
+      <c r="B106" t="n">
+        <v>1292.75</v>
+      </c>
+      <c r="C106" t="n">
+        <v>1176.25</v>
+      </c>
+      <c r="D106" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>131.58</v>
+      </c>
+      <c r="B107" t="n">
+        <v>1166.06</v>
+      </c>
+      <c r="C107" t="n">
+        <v>1176.21</v>
+      </c>
+      <c r="D107" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>131.48</v>
+      </c>
+      <c r="B108" t="n">
+        <v>1211.41</v>
+      </c>
+      <c r="C108" t="n">
+        <v>1176.2</v>
+      </c>
+      <c r="D108" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>131.38</v>
+      </c>
+      <c r="B109" t="n">
+        <v>1250.43</v>
+      </c>
+      <c r="C109" t="n">
+        <v>1176.15</v>
+      </c>
+      <c r="D109" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>131.28</v>
+      </c>
+      <c r="B110" t="n">
+        <v>1214.37</v>
+      </c>
+      <c r="C110" t="n">
+        <v>1176.11</v>
+      </c>
+      <c r="D110" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>131.18</v>
+      </c>
+      <c r="B111" t="n">
+        <v>1247.27</v>
+      </c>
+      <c r="C111" t="n">
+        <v>1176.06</v>
+      </c>
+      <c r="D111" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>131.08</v>
+      </c>
+      <c r="B112" t="n">
+        <v>1129.48</v>
+      </c>
+      <c r="C112" t="n">
+        <v>1176.05</v>
+      </c>
+      <c r="D112" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>130.98</v>
+      </c>
+      <c r="B113" t="n">
+        <v>1222.93</v>
+      </c>
+      <c r="C113" t="n">
+        <v>1176.05</v>
+      </c>
+      <c r="D113" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>130.88</v>
+      </c>
+      <c r="B114" t="n">
+        <v>1233.82</v>
+      </c>
+      <c r="C114" t="n">
+        <v>1176.01</v>
+      </c>
+      <c r="D114" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>130.78</v>
+      </c>
+      <c r="B115" t="n">
+        <v>1207.42</v>
+      </c>
+      <c r="C115" t="n">
+        <v>1175.97</v>
+      </c>
+      <c r="D115" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>130.68</v>
+      </c>
+      <c r="B116" t="n">
+        <v>1171.82</v>
+      </c>
+      <c r="C116" t="n">
+        <v>1175.96</v>
+      </c>
+      <c r="D116" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>130.58</v>
+      </c>
+      <c r="B117" t="n">
+        <v>1193.28</v>
+      </c>
+      <c r="C117" t="n">
+        <v>1175.96</v>
+      </c>
+      <c r="D117" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>130.48</v>
+      </c>
+      <c r="B118" t="n">
+        <v>1122.03</v>
+      </c>
+      <c r="C118" t="n">
+        <v>1175.97</v>
+      </c>
+      <c r="D118" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>130.38</v>
+      </c>
+      <c r="B119" t="n">
+        <v>1224.98</v>
+      </c>
+      <c r="C119" t="n">
+        <v>1175.97</v>
+      </c>
+      <c r="D119" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>130.28</v>
+      </c>
+      <c r="B120" t="n">
+        <v>1179.63</v>
+      </c>
+      <c r="C120" t="n">
+        <v>1175.95</v>
+      </c>
+      <c r="D120" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>130.18</v>
+      </c>
+      <c r="B121" t="n">
+        <v>1160.65</v>
+      </c>
+      <c r="C121" t="n">
+        <v>1160.65</v>
+      </c>
+      <c r="D121" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>130.08</v>
+      </c>
+      <c r="B122" t="n">
+        <v>1167.95</v>
+      </c>
+      <c r="C122" t="n">
+        <v>1167.95</v>
+      </c>
+      <c r="D122" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>129.98</v>
+      </c>
+      <c r="B123" t="n">
+        <v>1094.96</v>
+      </c>
+      <c r="C123" t="n">
+        <v>1094.96</v>
+      </c>
+      <c r="D123" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>129.88</v>
+      </c>
+      <c r="B124" t="n">
+        <v>1127.85</v>
+      </c>
+      <c r="C124" t="n">
+        <v>1127.85</v>
+      </c>
+      <c r="D124" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>129.78</v>
+      </c>
+      <c r="B125" t="n">
+        <v>1153.15</v>
+      </c>
+      <c r="C125" t="n">
+        <v>1153.15</v>
+      </c>
+      <c r="D125" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>129.68</v>
+      </c>
+      <c r="B126" t="n">
+        <v>1176.2</v>
+      </c>
+      <c r="C126" t="n">
+        <v>1176.2</v>
+      </c>
+      <c r="D126" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>129.58</v>
+      </c>
+      <c r="B127" t="n">
+        <v>1085.87</v>
+      </c>
+      <c r="C127" t="n">
+        <v>1085.87</v>
+      </c>
+      <c r="D127" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>129.48</v>
+      </c>
+      <c r="B128" t="n">
+        <v>1142.16</v>
+      </c>
+      <c r="C128" t="n">
+        <v>1142.16</v>
+      </c>
+      <c r="D128" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>129.38</v>
+      </c>
+      <c r="B129" t="n">
+        <v>1166.26</v>
+      </c>
+      <c r="C129" t="n">
+        <v>1166.26</v>
+      </c>
+      <c r="D129" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>129.28</v>
+      </c>
+      <c r="B130" t="n">
+        <v>1135.51</v>
+      </c>
+      <c r="C130" t="n">
+        <v>1135.51</v>
+      </c>
+      <c r="D130" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>129.18</v>
+      </c>
+      <c r="B131" t="n">
+        <v>1121.77</v>
+      </c>
+      <c r="C131" t="n">
+        <v>1121.77</v>
+      </c>
+      <c r="D131" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>129.08</v>
+      </c>
+      <c r="B132" t="n">
+        <v>1089.89</v>
+      </c>
+      <c r="C132" t="n">
+        <v>1089.89</v>
+      </c>
+      <c r="D132" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>128.98</v>
+      </c>
+      <c r="B133" t="n">
+        <v>1107.11</v>
+      </c>
+      <c r="C133" t="n">
+        <v>1107.11</v>
+      </c>
+      <c r="D133" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>128.88</v>
+      </c>
+      <c r="B134" t="n">
+        <v>1103.83</v>
+      </c>
+      <c r="C134" t="n">
+        <v>1103.83</v>
+      </c>
+      <c r="D134" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>128.78</v>
+      </c>
+      <c r="B135" t="n">
+        <v>1068.4</v>
+      </c>
+      <c r="C135" t="n">
+        <v>1068.4</v>
+      </c>
+      <c r="D135" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>128.68</v>
+      </c>
+      <c r="B136" t="n">
+        <v>1134.15</v>
+      </c>
+      <c r="C136" t="n">
+        <v>1134.15</v>
+      </c>
+      <c r="D136" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>128.58</v>
+      </c>
+      <c r="B137" t="n">
+        <v>1072.18</v>
+      </c>
+      <c r="C137" t="n">
+        <v>1072.18</v>
+      </c>
+      <c r="D137" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>128.48</v>
+      </c>
+      <c r="B138" t="n">
+        <v>1133.62</v>
+      </c>
+      <c r="C138" t="n">
+        <v>1133.62</v>
+      </c>
+      <c r="D138" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>128.38</v>
+      </c>
+      <c r="B139" t="n">
+        <v>1117.96</v>
+      </c>
+      <c r="C139" t="n">
+        <v>1117.96</v>
+      </c>
+      <c r="D139" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>128.28</v>
+      </c>
+      <c r="B140" t="n">
+        <v>1074.26</v>
+      </c>
+      <c r="C140" t="n">
+        <v>1074.26</v>
+      </c>
+      <c r="D140" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>128.18</v>
+      </c>
+      <c r="B141" t="n">
+        <v>1140.2</v>
+      </c>
+      <c r="C141" t="n">
+        <v>1140.2</v>
+      </c>
+      <c r="D141" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>128.08</v>
+      </c>
+      <c r="B142" t="n">
+        <v>1069.57</v>
+      </c>
+      <c r="C142" t="n">
+        <v>1069.57</v>
+      </c>
+      <c r="D142" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>127.98</v>
+      </c>
+      <c r="B143" t="n">
+        <v>1084.2</v>
+      </c>
+      <c r="C143" t="n">
+        <v>1084.2</v>
+      </c>
+      <c r="D143" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>127.88</v>
+      </c>
+      <c r="B144" t="n">
+        <v>1073.19</v>
+      </c>
+      <c r="C144" t="n">
+        <v>1073.19</v>
+      </c>
+      <c r="D144" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>127.78</v>
+      </c>
+      <c r="B145" t="n">
+        <v>1042.02</v>
+      </c>
+      <c r="C145" t="n">
+        <v>1042.02</v>
+      </c>
+      <c r="D145" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>127.68</v>
+      </c>
+      <c r="B146" t="n">
+        <v>1090.89</v>
+      </c>
+      <c r="C146" t="n">
+        <v>1090.89</v>
+      </c>
+      <c r="D146" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>127.58</v>
+      </c>
+      <c r="B147" t="n">
+        <v>1062.76</v>
+      </c>
+      <c r="C147" t="n">
+        <v>1062.76</v>
+      </c>
+      <c r="D147" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>127.48</v>
+      </c>
+      <c r="B148" t="n">
+        <v>1063.27</v>
+      </c>
+      <c r="C148" t="n">
+        <v>1063.27</v>
+      </c>
+      <c r="D148" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>127.38</v>
+      </c>
+      <c r="B149" t="n">
+        <v>1027.38</v>
+      </c>
+      <c r="C149" t="n">
+        <v>1027.38</v>
+      </c>
+      <c r="D149" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>127.28</v>
+      </c>
+      <c r="B150" t="n">
+        <v>1029.99</v>
+      </c>
+      <c r="C150" t="n">
+        <v>1029.99</v>
+      </c>
+      <c r="D150" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>127.18</v>
+      </c>
+      <c r="B151" t="n">
+        <v>1056.85</v>
+      </c>
+      <c r="C151" t="n">
+        <v>1056.85</v>
+      </c>
+      <c r="D151" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>127.08</v>
+      </c>
+      <c r="B152" t="n">
+        <v>1036.88</v>
+      </c>
+      <c r="C152" t="n">
+        <v>1036.88</v>
+      </c>
+      <c r="D152" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>126.98</v>
+      </c>
+      <c r="B153" t="n">
+        <v>1070.09</v>
+      </c>
+      <c r="C153" t="n">
+        <v>1070.09</v>
+      </c>
+      <c r="D153" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>126.88</v>
+      </c>
+      <c r="B154" t="n">
+        <v>1106.96</v>
+      </c>
+      <c r="C154" t="n">
+        <v>1106.96</v>
+      </c>
+      <c r="D154" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>126.78</v>
+      </c>
+      <c r="B155" t="n">
+        <v>1057.51</v>
+      </c>
+      <c r="C155" t="n">
+        <v>1057.51</v>
+      </c>
+      <c r="D155" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>126.68</v>
+      </c>
+      <c r="B156" t="n">
+        <v>1031.32</v>
+      </c>
+      <c r="C156" t="n">
+        <v>1031.32</v>
+      </c>
+      <c r="D156" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>126.58</v>
+      </c>
+      <c r="B157" t="n">
+        <v>1109.28</v>
+      </c>
+      <c r="C157" t="n">
+        <v>1109.28</v>
+      </c>
+      <c r="D157" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>126.48</v>
+      </c>
+      <c r="B158" t="n">
+        <v>1068.33</v>
+      </c>
+      <c r="C158" t="n">
+        <v>1068.33</v>
+      </c>
+      <c r="D158" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>126.38</v>
+      </c>
+      <c r="B159" t="n">
+        <v>1067.61</v>
+      </c>
+      <c r="C159" t="n">
+        <v>1067.61</v>
+      </c>
+      <c r="D159" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>126.28</v>
+      </c>
+      <c r="B160" t="n">
+        <v>1066.1</v>
+      </c>
+      <c r="C160" t="n">
+        <v>1066.1</v>
+      </c>
+      <c r="D160" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>126.18</v>
+      </c>
+      <c r="B161" t="n">
+        <v>1105</v>
+      </c>
+      <c r="C161" t="n">
+        <v>1105</v>
+      </c>
+      <c r="D161" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>126.08</v>
+      </c>
+      <c r="B162" t="n">
+        <v>1070.67</v>
+      </c>
+      <c r="C162" t="n">
+        <v>1070.67</v>
+      </c>
+      <c r="D162" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>